<commit_message>
Fix hydrogen BTU conversion factor
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21B2B95-D258-4E9E-9F97-083DCEE8197F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39315" yWindow="4335" windowWidth="20625" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39315" yWindow="4335" windowWidth="20625" windowHeight="14865"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
   <definedNames>
     <definedName name="gal_per_barrel">About!$A$84</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Michael Wang</author>
     <author>ywu</author>
@@ -51,7 +50,7 @@
     <author>A Elgowainy</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="G15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="G21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="G22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="G29" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="A43" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="A63" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B65" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
+    <comment ref="B65" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -260,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+    <comment ref="B66" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
+    <comment ref="D66" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -298,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
+    <comment ref="F66" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -311,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="G66" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="I66" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -337,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
+    <comment ref="B67" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -371,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
+    <comment ref="D67" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -384,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
+    <comment ref="F67" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
+    <comment ref="G67" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -410,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
+    <comment ref="I67" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -423,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
+    <comment ref="B68" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
+    <comment ref="D68" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
+    <comment ref="F68" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -483,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
+    <comment ref="G68" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="I68" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="B69" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -533,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
+    <comment ref="D69" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -546,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001D000000}">
+    <comment ref="F69" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -559,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001E000000}">
+    <comment ref="G69" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -572,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001F000000}">
+    <comment ref="I69" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000020000000}">
+    <comment ref="B70" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000021000000}">
+    <comment ref="D70" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -622,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000022000000}">
+    <comment ref="F70" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000023000000}">
+    <comment ref="G70" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000024000000}">
+    <comment ref="I70" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000025000000}">
+    <comment ref="B71" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -685,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000026000000}">
+    <comment ref="D71" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -698,7 +697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000027000000}">
+    <comment ref="F71" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -712,7 +711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000028000000}">
+    <comment ref="G71" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -725,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000029000000}">
+    <comment ref="I71" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002A000000}">
+    <comment ref="B72" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -762,7 +761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002B000000}">
+    <comment ref="D72" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002C000000}">
+    <comment ref="F72" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -788,7 +787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002D000000}">
+    <comment ref="G72" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -801,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002E000000}">
+    <comment ref="I72" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -814,7 +813,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002F000000}">
+    <comment ref="B73" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -838,7 +837,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000030000000}">
+    <comment ref="B74" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -862,7 +861,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000031000000}">
+    <comment ref="B76" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B77" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000032000000}">
+    <comment ref="B77" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -910,7 +909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B78" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000033000000}">
+    <comment ref="B78" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -934,7 +933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000034000000}">
+    <comment ref="B79" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -958,7 +957,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B80" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000035000000}">
+    <comment ref="B80" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -982,7 +981,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000036000000}">
+    <comment ref="B81" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1005,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000037000000}">
+    <comment ref="B82" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1030,7 +1029,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000038000000}">
+    <comment ref="B83" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1054,7 +1053,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000039000000}">
+    <comment ref="B84" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1078,7 +1077,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003A000000}">
+    <comment ref="B85" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1102,7 +1101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003B000000}">
+    <comment ref="B86" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1126,7 +1125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003C000000}">
+    <comment ref="B87" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1150,7 +1149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B88" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003D000000}">
+    <comment ref="B88" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1174,7 +1173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003E000000}">
+    <comment ref="A90" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2595,7 +2594,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="15">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -4019,14 +4018,14 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4056,22 +4055,22 @@
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Body: normal cell" xfId="48" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Body: normal cell" xfId="48"/>
+    <cellStyle name="Body: normal cell 2" xfId="57"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="61" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="43" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Footnotes: all except top row" xfId="52" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="45" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="43"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="59"/>
+    <cellStyle name="Footnotes: all except top row" xfId="52"/>
+    <cellStyle name="Footnotes: top row" xfId="45"/>
+    <cellStyle name="Footnotes: top row 2" xfId="55"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Header: top rows" xfId="51" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Header: bottom row" xfId="42"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
+    <cellStyle name="Header: top rows" xfId="51"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -4081,16 +4080,16 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 2" xfId="54"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="46" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Parent row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Parent row" xfId="46"/>
+    <cellStyle name="Parent row 2" xfId="56"/>
     <cellStyle name="Percent" xfId="62" builtinId="5"/>
-    <cellStyle name="Section Break" xfId="44" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Section Break: parent row" xfId="49" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Table title" xfId="50" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Table title 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Section Break" xfId="44"/>
+    <cellStyle name="Section Break: parent row" xfId="49"/>
+    <cellStyle name="Table title" xfId="50"/>
+    <cellStyle name="Table title 2" xfId="60"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -4122,7 +4121,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -4214,23 +4213,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4266,23 +4248,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4458,7 +4423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
@@ -4760,7 +4725,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A60" s="216" t="s">
+      <c r="A60" s="215" t="s">
         <v>383</v>
       </c>
       <c r="B60" s="200" t="s">
@@ -4792,7 +4757,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="216" t="s">
+      <c r="A64" s="215" t="s">
         <v>381</v>
       </c>
       <c r="B64" s="200" t="s">
@@ -4800,7 +4765,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="216" t="s">
+      <c r="A65" s="215" t="s">
         <v>348</v>
       </c>
       <c r="B65" s="200" t="s">
@@ -4828,7 +4793,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A69" s="216" t="s">
+      <c r="A69" s="215" t="s">
         <v>383</v>
       </c>
       <c r="B69" s="200" t="s">
@@ -4852,7 +4817,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A72" s="216" t="s">
+      <c r="A72" s="215" t="s">
         <v>382</v>
       </c>
       <c r="B72" s="200" t="s">
@@ -4868,7 +4833,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="216" t="s">
+      <c r="A74" s="215" t="s">
         <v>347</v>
       </c>
       <c r="B74" s="200" t="s">
@@ -4990,9 +4955,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{B531B8C1-CDDC-4ACF-AAC9-F602B8E5DC36}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{5B66228F-F935-4AD8-B4DD-34BC17502221}"/>
-    <hyperlink ref="B31" r:id="rId3" xr:uid="{9816D527-7FFC-4EB3-8075-F36973D92D26}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B31" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -5000,7 +4965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434DE0AC-D9FF-4E3B-BCFF-F5A0793B1649}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5099,7 +5064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83121717-82A7-4E9D-8C0F-4F196F1AB773}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5133,7 +5098,7 @@
       <c r="A5" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C5" s="215">
+      <c r="C5" s="214">
         <f>About!A86/1000</f>
         <v>3412.1414798968999</v>
       </c>
@@ -5198,7 +5163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11845,44 +11810,44 @@
     </row>
     <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="211" t="s">
+      <c r="B78" s="216" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="211"/>
-      <c r="D78" s="211"/>
-      <c r="E78" s="211"/>
-      <c r="F78" s="211"/>
-      <c r="G78" s="211"/>
-      <c r="H78" s="211"/>
-      <c r="I78" s="211"/>
-      <c r="J78" s="211"/>
-      <c r="K78" s="211"/>
-      <c r="L78" s="211"/>
-      <c r="M78" s="211"/>
-      <c r="N78" s="211"/>
-      <c r="O78" s="211"/>
-      <c r="P78" s="211"/>
-      <c r="Q78" s="211"/>
-      <c r="R78" s="211"/>
-      <c r="S78" s="211"/>
-      <c r="T78" s="211"/>
-      <c r="U78" s="211"/>
-      <c r="V78" s="211"/>
-      <c r="W78" s="211"/>
-      <c r="X78" s="211"/>
-      <c r="Y78" s="211"/>
-      <c r="Z78" s="211"/>
-      <c r="AA78" s="211"/>
-      <c r="AB78" s="211"/>
-      <c r="AC78" s="211"/>
-      <c r="AD78" s="211"/>
-      <c r="AE78" s="211"/>
-      <c r="AF78" s="211"/>
-      <c r="AG78" s="211"/>
-      <c r="AH78" s="211"/>
-      <c r="AI78" s="211"/>
-      <c r="AJ78" s="211"/>
-      <c r="AK78" s="211"/>
+      <c r="C78" s="216"/>
+      <c r="D78" s="216"/>
+      <c r="E78" s="216"/>
+      <c r="F78" s="216"/>
+      <c r="G78" s="216"/>
+      <c r="H78" s="216"/>
+      <c r="I78" s="216"/>
+      <c r="J78" s="216"/>
+      <c r="K78" s="216"/>
+      <c r="L78" s="216"/>
+      <c r="M78" s="216"/>
+      <c r="N78" s="216"/>
+      <c r="O78" s="216"/>
+      <c r="P78" s="216"/>
+      <c r="Q78" s="216"/>
+      <c r="R78" s="216"/>
+      <c r="S78" s="216"/>
+      <c r="T78" s="216"/>
+      <c r="U78" s="216"/>
+      <c r="V78" s="216"/>
+      <c r="W78" s="216"/>
+      <c r="X78" s="216"/>
+      <c r="Y78" s="216"/>
+      <c r="Z78" s="216"/>
+      <c r="AA78" s="216"/>
+      <c r="AB78" s="216"/>
+      <c r="AC78" s="216"/>
+      <c r="AD78" s="216"/>
+      <c r="AE78" s="216"/>
+      <c r="AF78" s="216"/>
+      <c r="AG78" s="216"/>
+      <c r="AH78" s="216"/>
+      <c r="AI78" s="216"/>
+      <c r="AJ78" s="216"/>
+      <c r="AK78" s="216"/>
     </row>
     <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="8" t="s">
@@ -11929,7 +11894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X163"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -16398,19 +16363,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100">
       <formula1>$D$100:$E$100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99">
       <formula1>"None, GWP, GTP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93">
       <formula1>$C$93:$D$93</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92">
       <formula1>"AR5/GWP,AR5/GTP,AR4/GWP,AR3/GWP,AR2/GWP,AR1/GWP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>"1,2"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16420,13 +16385,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -16971,7 +16938,7 @@
       <c r="A5" s="200" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="212">
+      <c r="B5" s="211">
         <f>39652608749183</f>
         <v>39652608749183</v>
       </c>
@@ -17433,139 +17400,139 @@
       <c r="A9" s="200" t="s">
         <v>324</v>
       </c>
-      <c r="B9" s="214">
+      <c r="B9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="C9" s="214">
+      <c r="C9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="D9" s="214">
+      <c r="D9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="E9" s="214">
+      <c r="E9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="F9" s="214">
+      <c r="F9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="G9" s="214">
+      <c r="G9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="H9" s="214">
+      <c r="H9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="I9" s="214">
+      <c r="I9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="J9" s="214">
+      <c r="J9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="K9" s="214">
+      <c r="K9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="L9" s="214">
+      <c r="L9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="M9" s="214">
+      <c r="M9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="N9" s="214">
+      <c r="N9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="O9" s="214">
+      <c r="O9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="P9" s="214">
+      <c r="P9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="Q9" s="214">
+      <c r="Q9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="R9" s="214">
+      <c r="R9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="S9" s="214">
+      <c r="S9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="T9" s="214">
+      <c r="T9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="U9" s="214">
+      <c r="U9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="V9" s="214">
+      <c r="V9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="W9" s="214">
+      <c r="W9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="X9" s="214">
+      <c r="X9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="Y9" s="214">
+      <c r="Y9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="Z9" s="214">
+      <c r="Z9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AA9" s="214">
+      <c r="AA9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AB9" s="214">
+      <c r="AB9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AC9" s="214">
+      <c r="AC9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AD9" s="214">
+      <c r="AD9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AE9" s="214">
+      <c r="AE9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AF9" s="214">
+      <c r="AF9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AG9" s="214">
+      <c r="AG9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AH9" s="214">
+      <c r="AH9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
-      <c r="AI9" s="214">
+      <c r="AI9" s="213">
         <f>'GREET1 Fuel_Specs'!$D$81*10^6*About!$A$88</f>
         <v>16244049954440</v>
       </c>
@@ -18950,139 +18917,139 @@
       <c r="A20" s="200" t="s">
         <v>360</v>
       </c>
-      <c r="B20" s="214">
+      <c r="B20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="C20" s="214">
+      <c r="C20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="D20" s="214">
+      <c r="D20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="E20" s="214">
+      <c r="E20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="F20" s="214">
+      <c r="F20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="G20" s="214">
+      <c r="G20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="H20" s="214">
+      <c r="H20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="I20" s="214">
+      <c r="I20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="J20" s="214">
+      <c r="J20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="K20" s="214">
+      <c r="K20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="L20" s="214">
+      <c r="L20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="M20" s="214">
+      <c r="M20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="N20" s="214">
+      <c r="N20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="O20" s="214">
+      <c r="O20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="P20" s="214">
+      <c r="P20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="Q20" s="214">
+      <c r="Q20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="R20" s="214">
+      <c r="R20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="S20" s="214">
+      <c r="S20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="T20" s="214">
+      <c r="T20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="U20" s="214">
+      <c r="U20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="V20" s="214">
+      <c r="V20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="W20" s="214">
+      <c r="W20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="X20" s="214">
+      <c r="X20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="Y20" s="214">
+      <c r="Y20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="Z20" s="214">
+      <c r="Z20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AA20" s="214">
+      <c r="AA20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AB20" s="214">
+      <c r="AB20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AC20" s="214">
+      <c r="AC20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AD20" s="214">
+      <c r="AD20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AE20" s="214">
+      <c r="AE20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AF20" s="214">
+      <c r="AF20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AG20" s="214">
+      <c r="AG20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AH20" s="214">
+      <c r="AH20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
-      <c r="AI20" s="214">
+      <c r="AI20" s="213">
         <f>'GREET1 Fuel_Specs'!$D$36*10^6*About!$A$89</f>
         <v>346024492638</v>
       </c>
@@ -19091,139 +19058,139 @@
       <c r="A21" s="200" t="s">
         <v>361</v>
       </c>
-      <c r="B21" s="214">
+      <c r="B21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="C21" s="214">
+      <c r="C21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="D21" s="214">
+      <c r="D21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="E21" s="214">
+      <c r="E21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="F21" s="214">
+      <c r="F21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="G21" s="214">
+      <c r="G21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="H21" s="214">
+      <c r="H21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="I21" s="214">
+      <c r="I21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="J21" s="214">
+      <c r="J21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="K21" s="214">
+      <c r="K21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="L21" s="214">
+      <c r="L21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="M21" s="214">
+      <c r="M21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="N21" s="214">
+      <c r="N21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="O21" s="214">
+      <c r="O21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="P21" s="214">
+      <c r="P21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="Q21" s="214">
+      <c r="Q21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="R21" s="214">
+      <c r="R21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="S21" s="214">
+      <c r="S21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="T21" s="214">
+      <c r="T21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="U21" s="214">
+      <c r="U21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="V21" s="214">
+      <c r="V21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="W21" s="214">
+      <c r="W21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="X21" s="214">
+      <c r="X21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="Y21" s="214">
+      <c r="Y21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="Z21" s="214">
+      <c r="Z21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AA21" s="214">
+      <c r="AA21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AB21" s="214">
+      <c r="AB21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AC21" s="214">
+      <c r="AC21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AD21" s="214">
+      <c r="AD21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AE21" s="214">
+      <c r="AE21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AF21" s="214">
+      <c r="AF21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AG21" s="214">
+      <c r="AG21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AH21" s="214">
+      <c r="AH21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
-      <c r="AI21" s="214">
+      <c r="AI21" s="213">
         <f>'GREET1 Fuel_Specs'!$D$90*10^6*About!$A$88</f>
         <v>12322693643480.453</v>
       </c>
@@ -19233,140 +19200,140 @@
         <v>357</v>
       </c>
       <c r="B22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="C22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="D22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="E22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="F22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="G22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="H22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="I22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="J22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="K22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="L22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="M22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="N22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="O22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="P22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Q22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="R22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="S22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="T22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="U22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="V22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="W22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="X22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Y22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Z22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AA22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AB22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AC22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AD22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AE22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AF22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AG22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AH22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AI22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
     </row>
   </sheetData>
@@ -19375,13 +19342,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -19501,139 +19470,139 @@
       <c r="A2" s="200" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="212">
+      <c r="B2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="C2" s="212">
+      <c r="C2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="D2" s="212">
+      <c r="D2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="E2" s="212">
+      <c r="E2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="F2" s="212">
+      <c r="F2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="G2" s="212">
+      <c r="G2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="H2" s="212">
+      <c r="H2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="I2" s="212">
+      <c r="I2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="J2" s="212">
+      <c r="J2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="K2" s="212">
+      <c r="K2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="L2" s="212">
+      <c r="L2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="M2" s="212">
+      <c r="M2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="N2" s="212">
+      <c r="N2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="O2" s="212">
+      <c r="O2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="P2" s="212">
+      <c r="P2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="Q2" s="212">
+      <c r="Q2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="R2" s="212">
+      <c r="R2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="S2" s="212">
+      <c r="S2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="T2" s="212">
+      <c r="T2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="U2" s="212">
+      <c r="U2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="V2" s="212">
+      <c r="V2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="W2" s="212">
+      <c r="W2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="X2" s="212">
+      <c r="X2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="Y2" s="212">
+      <c r="Y2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="Z2" s="212">
+      <c r="Z2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AA2" s="212">
+      <c r="AA2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AB2" s="212">
+      <c r="AB2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AC2" s="212">
+      <c r="AC2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AD2" s="212">
+      <c r="AD2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AE2" s="212">
+      <c r="AE2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AF2" s="212">
+      <c r="AF2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AG2" s="212">
+      <c r="AG2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AH2" s="212">
+      <c r="AH2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
-      <c r="AI2" s="212">
+      <c r="AI2" s="211">
         <f>About!$A$86</f>
         <v>3412141.4798968998</v>
       </c>
@@ -19924,7 +19893,7 @@
       <c r="A5" s="200" t="s">
         <v>349</v>
       </c>
-      <c r="B5" s="212">
+      <c r="B5" s="211">
         <f>39652608749.183</f>
         <v>39652608749.182999</v>
       </c>
@@ -20668,139 +20637,139 @@
       <c r="A11" s="200" t="s">
         <v>326</v>
       </c>
-      <c r="B11" s="213">
+      <c r="B11" s="212">
         <f>('AEO Table 73'!C19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="C11" s="212">
+      <c r="C11" s="211">
         <f>('AEO Table 73'!D19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="D11" s="212">
+      <c r="D11" s="211">
         <f>('AEO Table 73'!E19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="E11" s="212">
+      <c r="E11" s="211">
         <f>('AEO Table 73'!F19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="F11" s="212">
+      <c r="F11" s="211">
         <f>('AEO Table 73'!G19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="G11" s="212">
+      <c r="G11" s="211">
         <f>('AEO Table 73'!H19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="H11" s="212">
+      <c r="H11" s="211">
         <f>('AEO Table 73'!I19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="I11" s="212">
+      <c r="I11" s="211">
         <f>('AEO Table 73'!J19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="J11" s="212">
+      <c r="J11" s="211">
         <f>('AEO Table 73'!K19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="K11" s="212">
+      <c r="K11" s="211">
         <f>('AEO Table 73'!L19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="L11" s="212">
+      <c r="L11" s="211">
         <f>('AEO Table 73'!M19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="M11" s="212">
+      <c r="M11" s="211">
         <f>('AEO Table 73'!N19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="N11" s="212">
+      <c r="N11" s="211">
         <f>('AEO Table 73'!O19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="O11" s="212">
+      <c r="O11" s="211">
         <f>('AEO Table 73'!P19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="P11" s="212">
+      <c r="P11" s="211">
         <f>('AEO Table 73'!Q19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="Q11" s="212">
+      <c r="Q11" s="211">
         <f>('AEO Table 73'!R19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="R11" s="212">
+      <c r="R11" s="211">
         <f>('AEO Table 73'!S19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="S11" s="212">
+      <c r="S11" s="211">
         <f>('AEO Table 73'!T19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="T11" s="212">
+      <c r="T11" s="211">
         <f>('AEO Table 73'!U19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="U11" s="212">
+      <c r="U11" s="211">
         <f>('AEO Table 73'!V19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="V11" s="212">
+      <c r="V11" s="211">
         <f>('AEO Table 73'!W19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="W11" s="212">
+      <c r="W11" s="211">
         <f>('AEO Table 73'!X19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="X11" s="212">
+      <c r="X11" s="211">
         <f>('AEO Table 73'!Y19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="Y11" s="212">
+      <c r="Y11" s="211">
         <f>('AEO Table 73'!Z19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="Z11" s="212">
+      <c r="Z11" s="211">
         <f>('AEO Table 73'!AA19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AA11" s="212">
+      <c r="AA11" s="211">
         <f>('AEO Table 73'!AB19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AB11" s="212">
+      <c r="AB11" s="211">
         <f>('AEO Table 73'!AC19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AC11" s="212">
+      <c r="AC11" s="211">
         <f>('AEO Table 73'!AD19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AD11" s="212">
+      <c r="AD11" s="211">
         <f>('AEO Table 73'!AE19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AE11" s="212">
+      <c r="AE11" s="211">
         <f>('AEO Table 73'!AF19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AF11" s="212">
+      <c r="AF11" s="211">
         <f>('AEO Table 73'!AG19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AG11" s="212">
+      <c r="AG11" s="211">
         <f>('AEO Table 73'!AH19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AH11" s="212">
+      <c r="AH11" s="211">
         <f>('AEO Table 73'!AI19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
-      <c r="AI11" s="212">
+      <c r="AI11" s="211">
         <f>('AEO Table 73'!AJ19*10^6/gal_per_barrel)/About!$A$89</f>
         <v>36638.147582906618</v>
       </c>
@@ -22186,140 +22155,140 @@
         <v>357</v>
       </c>
       <c r="B22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="C22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="D22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="E22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="F22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="G22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="H22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="I22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="J22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="K22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="L22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="M22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="N22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="O22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="P22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Q22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="R22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="S22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="T22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="U22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="V22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="W22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="X22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Y22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Z22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AA22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AB22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AC22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AD22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AE22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AF22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AG22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AH22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AI22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
     </row>
   </sheetData>
@@ -22328,7 +22297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -23632,7 +23601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>

</xml_diff>

<commit_message>
Changed web-app/BCF small fuel output units of natural gas from MWh to thousand cubic feet
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FE9597-E708-4758-B395-F5F77ACC035E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39315" yWindow="4335" windowWidth="20625" windowHeight="14865"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
   <definedNames>
     <definedName name="gal_per_barrel">About!$A$84</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Michael Wang</author>
     <author>ywu</author>
@@ -50,7 +51,7 @@
     <author>A Elgowainy</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="0" shapeId="0">
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -100,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="1" shapeId="0">
+    <comment ref="G29" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="2" shapeId="0">
+    <comment ref="A43" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="3" shapeId="0">
+    <comment ref="A63" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B65" authorId="4" shapeId="0">
+    <comment ref="B65" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -245,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="4" shapeId="0">
+    <comment ref="B66" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -284,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="3" shapeId="0">
+    <comment ref="D66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -297,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F66" authorId="3" shapeId="0">
+    <comment ref="F66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -310,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G66" authorId="3" shapeId="0">
+    <comment ref="G66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -323,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I66" authorId="3" shapeId="0">
+    <comment ref="I66" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000010000000}">
       <text>
         <r>
           <rPr>
@@ -336,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="4" shapeId="0">
+    <comment ref="B67" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000011000000}">
       <text>
         <r>
           <rPr>
@@ -370,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="3" shapeId="0">
+    <comment ref="D67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000012000000}">
       <text>
         <r>
           <rPr>
@@ -383,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F67" authorId="3" shapeId="0">
+    <comment ref="F67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000013000000}">
       <text>
         <r>
           <rPr>
@@ -396,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G67" authorId="3" shapeId="0">
+    <comment ref="G67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000014000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I67" authorId="3" shapeId="0">
+    <comment ref="I67" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000015000000}">
       <text>
         <r>
           <rPr>
@@ -422,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="4" shapeId="0">
+    <comment ref="B68" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000016000000}">
       <text>
         <r>
           <rPr>
@@ -456,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="3" shapeId="0">
+    <comment ref="D68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000017000000}">
       <text>
         <r>
           <rPr>
@@ -469,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F68" authorId="3" shapeId="0">
+    <comment ref="F68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000018000000}">
       <text>
         <r>
           <rPr>
@@ -482,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G68" authorId="3" shapeId="0">
+    <comment ref="G68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000019000000}">
       <text>
         <r>
           <rPr>
@@ -495,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I68" authorId="3" shapeId="0">
+    <comment ref="I68" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -508,7 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="4" shapeId="0">
+    <comment ref="B69" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -532,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="3" shapeId="0">
+    <comment ref="D69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -545,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F69" authorId="3" shapeId="0">
+    <comment ref="F69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -558,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G69" authorId="3" shapeId="0">
+    <comment ref="G69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -571,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I69" authorId="3" shapeId="0">
+    <comment ref="I69" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -584,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="4" shapeId="0">
+    <comment ref="B70" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000020000000}">
       <text>
         <r>
           <rPr>
@@ -608,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D70" authorId="3" shapeId="0">
+    <comment ref="D70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000021000000}">
       <text>
         <r>
           <rPr>
@@ -621,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F70" authorId="3" shapeId="0">
+    <comment ref="F70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000022000000}">
       <text>
         <r>
           <rPr>
@@ -634,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="3" shapeId="0">
+    <comment ref="G70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000023000000}">
       <text>
         <r>
           <rPr>
@@ -647,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I70" authorId="3" shapeId="0">
+    <comment ref="I70" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000024000000}">
       <text>
         <r>
           <rPr>
@@ -660,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="4" shapeId="0">
+    <comment ref="B71" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000025000000}">
       <text>
         <r>
           <rPr>
@@ -684,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D71" authorId="3" shapeId="0">
+    <comment ref="D71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000026000000}">
       <text>
         <r>
           <rPr>
@@ -697,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F71" authorId="3" shapeId="0">
+    <comment ref="F71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000027000000}">
       <text>
         <r>
           <rPr>
@@ -711,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G71" authorId="3" shapeId="0">
+    <comment ref="G71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000028000000}">
       <text>
         <r>
           <rPr>
@@ -724,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I71" authorId="3" shapeId="0">
+    <comment ref="I71" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-000029000000}">
       <text>
         <r>
           <rPr>
@@ -737,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="4" shapeId="0">
+    <comment ref="B72" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -761,7 +762,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="3" shapeId="0">
+    <comment ref="D72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -774,7 +775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F72" authorId="3" shapeId="0">
+    <comment ref="F72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -787,7 +788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G72" authorId="3" shapeId="0">
+    <comment ref="G72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -800,7 +801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I72" authorId="3" shapeId="0">
+    <comment ref="I72" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -813,7 +814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="4" shapeId="0">
+    <comment ref="B73" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -837,7 +838,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="4" shapeId="0">
+    <comment ref="B74" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000030000000}">
       <text>
         <r>
           <rPr>
@@ -861,7 +862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="4" shapeId="0">
+    <comment ref="B76" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000031000000}">
       <text>
         <r>
           <rPr>
@@ -885,7 +886,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B77" authorId="4" shapeId="0">
+    <comment ref="B77" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000032000000}">
       <text>
         <r>
           <rPr>
@@ -909,7 +910,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B78" authorId="4" shapeId="0">
+    <comment ref="B78" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000033000000}">
       <text>
         <r>
           <rPr>
@@ -933,7 +934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="4" shapeId="0">
+    <comment ref="B79" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000034000000}">
       <text>
         <r>
           <rPr>
@@ -957,7 +958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B80" authorId="4" shapeId="0">
+    <comment ref="B80" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000035000000}">
       <text>
         <r>
           <rPr>
@@ -981,7 +982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="4" shapeId="0">
+    <comment ref="B81" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000036000000}">
       <text>
         <r>
           <rPr>
@@ -1005,7 +1006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="4" shapeId="0">
+    <comment ref="B82" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000037000000}">
       <text>
         <r>
           <rPr>
@@ -1029,7 +1030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="4" shapeId="0">
+    <comment ref="B83" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000038000000}">
       <text>
         <r>
           <rPr>
@@ -1053,7 +1054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="4" shapeId="0">
+    <comment ref="B84" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000039000000}">
       <text>
         <r>
           <rPr>
@@ -1077,7 +1078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="4" shapeId="0">
+    <comment ref="B85" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -1101,7 +1102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="4" shapeId="0">
+    <comment ref="B86" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -1125,7 +1126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="4" shapeId="0">
+    <comment ref="B87" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -1149,7 +1150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B88" authorId="4" shapeId="0">
+    <comment ref="B88" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -1173,7 +1174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A90" authorId="0" shapeId="0">
+    <comment ref="A90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="460">
   <si>
     <t>(from physical units to million Btu)</t>
   </si>
@@ -2590,11 +2591,17 @@
   <si>
     <t>Some units differ from the U.S. model, in which case the appropriate conversions were made.</t>
   </si>
+  <si>
+    <t>billion cubic meter to thousand cubic meter</t>
+  </si>
+  <si>
+    <t>thousand cubic meters (tcm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="15">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -4055,22 +4062,22 @@
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Body: normal cell" xfId="48"/>
-    <cellStyle name="Body: normal cell 2" xfId="57"/>
+    <cellStyle name="Body: normal cell" xfId="48" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="61" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="43"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="59"/>
-    <cellStyle name="Footnotes: all except top row" xfId="52"/>
-    <cellStyle name="Footnotes: top row" xfId="45"/>
-    <cellStyle name="Footnotes: top row 2" xfId="55"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="43" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="52" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="45" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="42"/>
-    <cellStyle name="Header: bottom row 2" xfId="58"/>
-    <cellStyle name="Header: top rows" xfId="51"/>
+    <cellStyle name="Header: bottom row" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Header: top rows" xfId="51" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -4080,16 +4087,16 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="54"/>
+    <cellStyle name="Normal 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="46"/>
-    <cellStyle name="Parent row 2" xfId="56"/>
+    <cellStyle name="Parent row" xfId="46" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Parent row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Percent" xfId="62" builtinId="5"/>
-    <cellStyle name="Section Break" xfId="44"/>
-    <cellStyle name="Section Break: parent row" xfId="49"/>
-    <cellStyle name="Table title" xfId="50"/>
-    <cellStyle name="Table title 2" xfId="60"/>
+    <cellStyle name="Section Break" xfId="44" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="49" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Table title" xfId="50" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Table title 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -4121,7 +4128,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -4213,6 +4220,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4248,6 +4272,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4423,44 +4464,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="37.3984375" customWidth="1"/>
+    <col min="1" max="1" width="37.40625" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="39.3984375" customWidth="1"/>
+    <col min="3" max="3" width="39.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -4468,252 +4509,252 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A8" s="1"/>
       <c r="B8" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A13" s="1"/>
       <c r="B13" s="196" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A15" s="1"/>
       <c r="B15" s="3">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B20" s="196" t="s">
         <v>435</v>
       </c>
       <c r="C20" s="202"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B22" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B23" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B24" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B25" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B27" s="196" t="s">
         <v>434</v>
       </c>
       <c r="C27" s="202"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B28" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B29" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B30" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B31" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B32" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A37" s="197" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A38" s="197" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A39" s="197" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A40" s="203" t="s">
         <v>457</v>
       </c>
       <c r="B40" s="200"/>
       <c r="C40" s="200"/>
     </row>
-    <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>308</v>
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>309</v>
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A45" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A46" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A47" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A48" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A49" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A50" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A52" s="2" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A53" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A54" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A56" s="1" t="s">
         <v>420</v>
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A57" s="1"/>
       <c r="G57"/>
     </row>
-    <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A58" s="198" t="s">
         <v>330</v>
       </c>
       <c r="B58" s="199"/>
     </row>
-    <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A59" s="203" t="s">
         <v>342</v>
       </c>
@@ -4724,7 +4765,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" s="2" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A60" s="215" t="s">
         <v>383</v>
       </c>
@@ -4732,7 +4773,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A61" s="203" t="s">
         <v>323</v>
       </c>
@@ -4740,7 +4781,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A62" s="197" t="s">
         <v>357</v>
       </c>
@@ -4748,7 +4789,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" s="2" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A63" s="201" t="s">
         <v>378</v>
       </c>
@@ -4756,7 +4797,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A64" s="215" t="s">
         <v>381</v>
       </c>
@@ -4764,7 +4805,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A65" s="215" t="s">
         <v>348</v>
       </c>
@@ -4775,16 +4816,16 @@
         <v>351</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A66" s="201"/>
     </row>
-    <row r="67" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A67" s="198" t="s">
         <v>333</v>
       </c>
       <c r="B67" s="199"/>
     </row>
-    <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A68" s="203" t="s">
         <v>342</v>
       </c>
@@ -4792,7 +4833,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" s="2" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A69" s="215" t="s">
         <v>383</v>
       </c>
@@ -4800,15 +4841,15 @@
         <v>415</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A70" s="203" t="s">
         <v>323</v>
       </c>
       <c r="B70" s="200" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A71" s="197" t="s">
         <v>357</v>
       </c>
@@ -4816,7 +4857,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" s="2" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A72" s="215" t="s">
         <v>382</v>
       </c>
@@ -4824,7 +4865,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A73" s="201" t="s">
         <v>379</v>
       </c>
@@ -4832,7 +4873,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A74" s="215" t="s">
         <v>347</v>
       </c>
@@ -4840,37 +4881,37 @@
         <v>414</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="76" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A76" s="198" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A77" s="200" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="79" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A79" s="198" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A80" s="200" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A83" s="196" t="s">
         <v>316</v>
       </c>
       <c r="B83" s="202"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A84" s="200">
         <v>42</v>
       </c>
@@ -4879,7 +4920,7 @@
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A85" s="2">
         <v>158.9873</v>
       </c>
@@ -4888,7 +4929,7 @@
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A86" s="2">
         <v>3412141.4798968998</v>
       </c>
@@ -4897,7 +4938,7 @@
       </c>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A87" s="2">
         <f>2.5219021687207*10^-8</f>
         <v>2.5219021687207001E-8</v>
@@ -4906,7 +4947,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A88" s="207">
         <v>0.90718474000000004</v>
       </c>
@@ -4915,7 +4956,7 @@
       </c>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A89" s="207">
         <v>3.7854117999999999</v>
       </c>
@@ -4924,7 +4965,7 @@
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A90" s="2">
         <v>235.214583</v>
       </c>
@@ -4933,31 +4974,31 @@
       </c>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A92" s="201"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G96" s="2"/>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.75">
       <c r="G105" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
-    <hyperlink ref="B31" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -4965,29 +5006,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.3984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.40625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.40625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.58984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="92.73046875" customWidth="1"/>
+    <col min="9" max="9" width="92.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B2" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.75">
       <c r="C3" s="1" t="s">
         <v>424</v>
       </c>
@@ -5002,7 +5043,7 @@
       </c>
       <c r="I3" s="201"/>
     </row>
-    <row r="4" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B4" s="2" t="s">
         <v>322</v>
       </c>
@@ -5022,7 +5063,7 @@
         <v>25306715975902.305</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B5" s="2" t="s">
         <v>329</v>
       </c>
@@ -5042,7 +5083,7 @@
         <v>11279023225214.885</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" ht="59" x14ac:dyDescent="0.75">
       <c r="B7" s="209" t="s">
         <v>451</v>
       </c>
@@ -5053,7 +5094,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>429</v>
       </c>
@@ -5064,37 +5105,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="12.265625" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.58984375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" s="208" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>450</v>
       </c>
@@ -5103,13 +5144,13 @@
         <v>3412.1414798968999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>439</v>
       </c>
@@ -5117,7 +5158,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>275</v>
       </c>
@@ -5129,7 +5170,7 @@
         <v>36953.492227283423</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>441</v>
       </c>
@@ -5142,7 +5183,7 @@
         <v>36953476200000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>442</v>
       </c>
@@ -5154,8 +5195,17 @@
         <v>3412141.4798968998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>458</v>
+      </c>
+      <c r="D13">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5163,7 +5213,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5174,14 +5224,14 @@
       <selection pane="bottomRight" activeCell="O85" sqref="O85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="20.86328125" style="7" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.73046875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="7" customWidth="1"/>
     <col min="3" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="B1" s="18" t="s">
         <v>377</v>
       </c>
@@ -5288,8 +5338,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C3" s="20" t="s">
         <v>121</v>
       </c>
@@ -5300,7 +5350,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C4" s="20" t="s">
         <v>120</v>
       </c>
@@ -5313,7 +5363,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C5" s="20" t="s">
         <v>118</v>
       </c>
@@ -5324,7 +5374,7 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C6" s="20" t="s">
         <v>117</v>
       </c>
@@ -5335,7 +5385,7 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A10" s="9" t="s">
         <v>116</v>
       </c>
@@ -5343,12 +5393,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B11" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B12" s="18" t="s">
         <v>2</v>
       </c>
@@ -5458,7 +5508,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
@@ -5568,17 +5618,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.65">
       <c r="B14" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B15" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A16" s="9" t="s">
         <v>114</v>
       </c>
@@ -5691,7 +5741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A17" s="9" t="s">
         <v>113</v>
       </c>
@@ -5804,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="9" t="s">
         <v>112</v>
       </c>
@@ -5917,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A19" s="9" t="s">
         <v>111</v>
       </c>
@@ -6030,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A20" s="9" t="s">
         <v>110</v>
       </c>
@@ -6143,7 +6193,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A21" s="9" t="s">
         <v>109</v>
       </c>
@@ -6256,7 +6306,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A22" s="9" t="s">
         <v>108</v>
       </c>
@@ -6369,7 +6419,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A23" s="9" t="s">
         <v>107</v>
       </c>
@@ -6482,7 +6532,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A24" s="9" t="s">
         <v>106</v>
       </c>
@@ -6595,7 +6645,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A25" s="9" t="s">
         <v>105</v>
       </c>
@@ -6708,7 +6758,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A26" s="9" t="s">
         <v>104</v>
       </c>
@@ -6821,7 +6871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A27" s="9" t="s">
         <v>103</v>
       </c>
@@ -6934,7 +6984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A28" s="9" t="s">
         <v>102</v>
       </c>
@@ -7047,7 +7097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A29" s="9" t="s">
         <v>100</v>
       </c>
@@ -7160,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A30" s="9" t="s">
         <v>99</v>
       </c>
@@ -7273,7 +7323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A31" s="9" t="s">
         <v>98</v>
       </c>
@@ -7386,7 +7436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A32" s="9" t="s">
         <v>97</v>
       </c>
@@ -7499,7 +7549,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A33" s="9" t="s">
         <v>96</v>
       </c>
@@ -7612,7 +7662,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A34" s="9" t="s">
         <v>95</v>
       </c>
@@ -7725,7 +7775,7 @@
         <v>-2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A35" s="9" t="s">
         <v>370</v>
       </c>
@@ -7838,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A36" s="9" t="s">
         <v>368</v>
       </c>
@@ -7951,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A37" s="9" t="s">
         <v>94</v>
       </c>
@@ -8064,7 +8114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A38" s="9" t="s">
         <v>93</v>
       </c>
@@ -8177,7 +8227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A39" s="9" t="s">
         <v>92</v>
       </c>
@@ -8290,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A40" s="9" t="s">
         <v>91</v>
       </c>
@@ -8403,7 +8453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A41" s="9" t="s">
         <v>90</v>
       </c>
@@ -8516,7 +8566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A42" s="9" t="s">
         <v>89</v>
       </c>
@@ -8629,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A43" s="9" t="s">
         <v>88</v>
       </c>
@@ -8742,7 +8792,7 @@
         <v>1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A44" s="9" t="s">
         <v>87</v>
       </c>
@@ -8855,7 +8905,7 @@
         <v>-4.8299999999999998E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A45" s="9" t="s">
         <v>86</v>
       </c>
@@ -8968,7 +9018,7 @@
         <v>-3.1150000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A46" s="9" t="s">
         <v>85</v>
       </c>
@@ -9081,12 +9131,12 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B47" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A48" s="9" t="s">
         <v>84</v>
       </c>
@@ -9199,7 +9249,7 @@
         <v>-2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A49" s="9" t="s">
         <v>83</v>
       </c>
@@ -9312,7 +9362,7 @@
         <v>-3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A50" s="9" t="s">
         <v>82</v>
       </c>
@@ -9425,7 +9475,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A51" s="9" t="s">
         <v>81</v>
       </c>
@@ -9538,12 +9588,12 @@
         <v>-2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B53" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A54" s="9" t="s">
         <v>80</v>
       </c>
@@ -9656,7 +9706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A55" s="9" t="s">
         <v>79</v>
       </c>
@@ -9769,7 +9819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A56" s="9" t="s">
         <v>78</v>
       </c>
@@ -9882,7 +9932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A57" s="9" t="s">
         <v>77</v>
       </c>
@@ -9995,7 +10045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A58" s="9" t="s">
         <v>76</v>
       </c>
@@ -10108,7 +10158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="9" t="s">
         <v>75</v>
       </c>
@@ -10221,7 +10271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A60" s="9" t="s">
         <v>74</v>
       </c>
@@ -10334,12 +10384,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B62" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A63" s="9" t="s">
         <v>73</v>
       </c>
@@ -10452,7 +10502,7 @@
         <v>-1.4100000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A64" s="9" t="s">
         <v>72</v>
       </c>
@@ -10565,7 +10615,7 @@
         <v>-1.0139999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A65" s="9" t="s">
         <v>71</v>
       </c>
@@ -10678,7 +10728,7 @@
         <v>-2.1699999999999999E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A66" s="9" t="s">
         <v>70</v>
       </c>
@@ -10791,7 +10841,7 @@
         <v>2.8499999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A67" s="9" t="s">
         <v>69</v>
       </c>
@@ -10904,7 +10954,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A68" s="9" t="s">
         <v>68</v>
       </c>
@@ -11017,7 +11067,7 @@
         <v>-5.5000000000000002E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A69" s="9" t="s">
         <v>67</v>
       </c>
@@ -11130,7 +11180,7 @@
         <v>-9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A70" s="9" t="s">
         <v>66</v>
       </c>
@@ -11243,7 +11293,7 @@
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A71" s="9" t="s">
         <v>65</v>
       </c>
@@ -11356,7 +11406,7 @@
         <v>5.7700000000000004E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A72" s="9" t="s">
         <v>64</v>
       </c>
@@ -11469,7 +11519,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A73" s="9" t="s">
         <v>63</v>
       </c>
@@ -11582,7 +11632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A74" s="9" t="s">
         <v>62</v>
       </c>
@@ -11695,7 +11745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A76" s="9" t="s">
         <v>61</v>
       </c>
@@ -11808,8 +11858,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8"/>
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B78" s="216" t="s">
         <v>57</v>
       </c>
@@ -11849,37 +11899,37 @@
       <c r="AJ78" s="216"/>
       <c r="AK78" s="216"/>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B79" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B80" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B81" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B82" s="8" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B83" s="8" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B84" s="8" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B85" s="8" t="s">
         <v>363</v>
       </c>
@@ -11894,47 +11944,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X163"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="33.1328125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.40625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58984375" style="22" customWidth="1"/>
     <col min="4" max="4" width="12.86328125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3984375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.73046875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.40625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.40625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1328125" style="22"/>
-    <col min="11" max="11" width="10.3984375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.40625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="12.40625" style="22" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="9.1328125" style="22"/>
     <col min="15" max="15" width="12.86328125" style="22" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="9.1328125" style="22"/>
-    <col min="19" max="19" width="10.3984375" style="22" customWidth="1"/>
+    <col min="19" max="19" width="10.40625" style="22" customWidth="1"/>
     <col min="20" max="22" width="9.1328125" style="22"/>
-    <col min="23" max="23" width="10.73046875" style="22" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" style="22" customWidth="1"/>
     <col min="24" max="16384" width="9.1328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.75">
       <c r="A1" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A2" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="24" t="s">
         <v>126</v>
       </c>
@@ -11957,7 +12007,7 @@
       </c>
       <c r="I3" s="29"/>
     </row>
-    <row r="4" spans="1:23" ht="26.65" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" ht="26.75" x14ac:dyDescent="0.75">
       <c r="A4" s="30"/>
       <c r="B4" s="31" t="s">
         <v>302</v>
@@ -11982,7 +12032,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A5" s="35" t="s">
         <v>137</v>
       </c>
@@ -11999,7 +12049,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A6" s="41" t="s">
         <v>139</v>
       </c>
@@ -12024,7 +12074,7 @@
       <c r="T6" s="47"/>
       <c r="V6" s="47"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A7" s="48" t="s">
         <v>142</v>
       </c>
@@ -12061,7 +12111,7 @@
       <c r="V7" s="55"/>
       <c r="W7" s="55"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A8" s="48" t="s">
         <v>143</v>
       </c>
@@ -12098,7 +12148,7 @@
       <c r="V8" s="55"/>
       <c r="W8" s="55"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A9" s="48" t="s">
         <v>144</v>
       </c>
@@ -12135,7 +12185,7 @@
       <c r="V9" s="55"/>
       <c r="W9" s="55"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A10" s="48" t="s">
         <v>145</v>
       </c>
@@ -12168,7 +12218,7 @@
       <c r="V10" s="55"/>
       <c r="W10" s="55"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A11" s="48" t="s">
         <v>146</v>
       </c>
@@ -12209,7 +12259,7 @@
       <c r="V11" s="55"/>
       <c r="W11" s="55"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A12" s="48" t="s">
         <v>147</v>
       </c>
@@ -12246,7 +12296,7 @@
       <c r="R12" s="55"/>
       <c r="S12" s="55"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A13" s="22" t="s">
         <v>148</v>
       </c>
@@ -12275,7 +12325,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A14" s="22" t="s">
         <v>149</v>
       </c>
@@ -12304,7 +12354,7 @@
         <v>0.93726057101554017</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A15" s="48" t="s">
         <v>150</v>
       </c>
@@ -12342,7 +12392,7 @@
       <c r="V15" s="65"/>
       <c r="W15" s="61"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A16" s="48" t="s">
         <v>151</v>
       </c>
@@ -12376,7 +12426,7 @@
       <c r="V16" s="65"/>
       <c r="W16" s="61"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A17" s="48" t="s">
         <v>152</v>
       </c>
@@ -12414,7 +12464,7 @@
       <c r="V17" s="65"/>
       <c r="W17" s="61"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A18" s="48" t="s">
         <v>153</v>
       </c>
@@ -12448,7 +12498,7 @@
       <c r="V18" s="65"/>
       <c r="W18" s="61"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A19" s="48" t="s">
         <v>154</v>
       </c>
@@ -12482,7 +12532,7 @@
       <c r="M19" s="65"/>
       <c r="N19" s="61"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A20" s="67" t="s">
         <v>303</v>
       </c>
@@ -12513,7 +12563,7 @@
       <c r="O20" s="55"/>
       <c r="W20" s="61"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A21" s="68" t="s">
         <v>395</v>
       </c>
@@ -12540,7 +12590,7 @@
       </c>
       <c r="I21" s="54"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A22" s="48" t="s">
         <v>155</v>
       </c>
@@ -12569,7 +12619,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A23" s="48" t="s">
         <v>156</v>
       </c>
@@ -12598,7 +12648,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A24" s="48" t="s">
         <v>157</v>
       </c>
@@ -12627,7 +12677,7 @@
         <v>0.93476175247841387</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A25" s="70" t="s">
         <v>396</v>
       </c>
@@ -12656,7 +12706,7 @@
         <v>0.93404711473172097</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A26" s="71" t="s">
         <v>158</v>
       </c>
@@ -12685,7 +12735,7 @@
         <v>0.93500003751584637</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A27" s="71" t="s">
         <v>159</v>
       </c>
@@ -12714,7 +12764,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A28" s="71" t="s">
         <v>160</v>
       </c>
@@ -12744,7 +12794,7 @@
       </c>
       <c r="J28" s="73"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A29" s="71" t="s">
         <v>161</v>
       </c>
@@ -12773,7 +12823,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A30" s="71" t="s">
         <v>162</v>
       </c>
@@ -12802,7 +12852,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A31" s="71" t="s">
         <v>163</v>
       </c>
@@ -12832,7 +12882,7 @@
       </c>
       <c r="J31" s="73"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A32" s="71" t="s">
         <v>164</v>
       </c>
@@ -12861,7 +12911,7 @@
         <v>0.90299302022950434</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A33" s="71" t="s">
         <v>165</v>
       </c>
@@ -12891,7 +12941,7 @@
       </c>
       <c r="J33" s="73"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A34" s="71" t="s">
         <v>166</v>
       </c>
@@ -12920,7 +12970,7 @@
         <v>0.92867915675168411</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A35" s="71" t="s">
         <v>167</v>
       </c>
@@ -12950,7 +13000,7 @@
       </c>
       <c r="J35" s="73"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A36" s="71" t="s">
         <v>168</v>
       </c>
@@ -12980,7 +13030,7 @@
       </c>
       <c r="J36" s="73"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A37" s="71" t="s">
         <v>169</v>
       </c>
@@ -13010,7 +13060,7 @@
       </c>
       <c r="J37" s="73"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A38" s="71" t="s">
         <v>170</v>
       </c>
@@ -13040,7 +13090,7 @@
       </c>
       <c r="J38" s="73"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A39" s="71" t="s">
         <v>171</v>
       </c>
@@ -13071,7 +13121,7 @@
       <c r="J39" s="73"/>
       <c r="K39" s="73"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A40" s="71" t="s">
         <v>172</v>
       </c>
@@ -13102,7 +13152,7 @@
       <c r="J40" s="73"/>
       <c r="K40" s="73"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A41" s="71" t="s">
         <v>173</v>
       </c>
@@ -13132,7 +13182,7 @@
       </c>
       <c r="K41" s="73"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A42" s="70" t="s">
         <v>174</v>
       </c>
@@ -13162,7 +13212,7 @@
       </c>
       <c r="K42" s="73"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A43" s="70" t="s">
         <v>175</v>
       </c>
@@ -13192,7 +13242,7 @@
       </c>
       <c r="K43" s="73"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A44" s="71" t="s">
         <v>176</v>
       </c>
@@ -13222,7 +13272,7 @@
       </c>
       <c r="K44" s="73"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A45" s="22" t="s">
         <v>177</v>
       </c>
@@ -13251,7 +13301,7 @@
         <v>0.93361506882395562</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A46" s="71" t="s">
         <v>178</v>
       </c>
@@ -13281,7 +13331,7 @@
       </c>
       <c r="K46" s="73"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A47" s="48" t="s">
         <v>397</v>
       </c>
@@ -13310,7 +13360,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A48" s="48" t="s">
         <v>179</v>
       </c>
@@ -13339,7 +13389,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A49" s="48" t="s">
         <v>180</v>
       </c>
@@ -13369,7 +13419,7 @@
       </c>
       <c r="J49" s="73"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A50" s="48" t="s">
         <v>181</v>
       </c>
@@ -13399,7 +13449,7 @@
       </c>
       <c r="J50" s="73"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A51" s="48" t="s">
         <v>182</v>
       </c>
@@ -13429,7 +13479,7 @@
       </c>
       <c r="J51" s="73"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A52" s="48" t="s">
         <v>183</v>
       </c>
@@ -13459,7 +13509,7 @@
       </c>
       <c r="J52" s="73"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A53" s="48" t="s">
         <v>184</v>
       </c>
@@ -13489,7 +13539,7 @@
       </c>
       <c r="J53" s="73"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A54" s="48" t="s">
         <v>185</v>
       </c>
@@ -13519,7 +13569,7 @@
       </c>
       <c r="J54" s="73"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A55" s="48" t="s">
         <v>186</v>
       </c>
@@ -13549,7 +13599,7 @@
       </c>
       <c r="J55" s="73"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A56" s="67" t="s">
         <v>187</v>
       </c>
@@ -13578,7 +13628,7 @@
         <v>0.92157077225989936</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A57" s="48" t="s">
         <v>188</v>
       </c>
@@ -13605,7 +13655,7 @@
         <v>0.92932939503336609</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A58" s="41" t="s">
         <v>189</v>
       </c>
@@ -13634,7 +13684,7 @@
         <v>0.93722267739953979</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A59" s="48" t="s">
         <v>191</v>
       </c>
@@ -13657,7 +13707,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A60" s="67" t="s">
         <v>194</v>
       </c>
@@ -13686,7 +13736,7 @@
         <v>0.90266299357208446</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A61" s="48" t="s">
         <v>195</v>
       </c>
@@ -13716,7 +13766,7 @@
       </c>
       <c r="L61" s="47"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A62" s="48" t="s">
         <v>196</v>
       </c>
@@ -13745,7 +13795,7 @@
         <v>0.84548104956268222</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A63" s="71" t="s">
         <v>197</v>
       </c>
@@ -13766,7 +13816,7 @@
       </c>
       <c r="I63" s="54"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A64" s="41" t="s">
         <v>190</v>
       </c>
@@ -13796,7 +13846,7 @@
       </c>
       <c r="K64" s="47"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A65" s="67" t="s">
         <v>198</v>
       </c>
@@ -13817,7 +13867,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A66" s="68" t="s">
         <v>200</v>
       </c>
@@ -13843,7 +13893,7 @@
       <c r="I66" s="94"/>
       <c r="K66" s="95"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A67" s="68" t="s">
         <v>201</v>
       </c>
@@ -13871,7 +13921,7 @@
       </c>
       <c r="K67" s="95"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A68" s="68" t="s">
         <v>202</v>
       </c>
@@ -13899,7 +13949,7 @@
       </c>
       <c r="K68" s="95"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A69" s="68" t="s">
         <v>203</v>
       </c>
@@ -13927,7 +13977,7 @@
       </c>
       <c r="K69" s="95"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A70" s="68" t="s">
         <v>204</v>
       </c>
@@ -13956,7 +14006,7 @@
       <c r="K70" s="95"/>
       <c r="M70" s="73"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A71" s="71" t="s">
         <v>205</v>
       </c>
@@ -13985,7 +14035,7 @@
       <c r="K71" s="95"/>
       <c r="L71" s="95"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A72" s="70" t="s">
         <v>206</v>
       </c>
@@ -14013,7 +14063,7 @@
       </c>
       <c r="K72" s="95"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A73" s="48" t="s">
         <v>207</v>
       </c>
@@ -14040,7 +14090,7 @@
         <v>0.94242199100000001</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" ht="12.65" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A74" s="48" t="s">
         <v>208</v>
       </c>
@@ -14068,7 +14118,7 @@
       </c>
       <c r="K74" s="97"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A75" s="48" t="s">
         <v>398</v>
       </c>
@@ -14096,7 +14146,7 @@
       </c>
       <c r="K75" s="97"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A76" s="48" t="s">
         <v>209</v>
       </c>
@@ -14123,7 +14173,7 @@
         <v>0.93173565722585328</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A77" s="70" t="s">
         <v>210</v>
       </c>
@@ -14152,7 +14202,7 @@
       <c r="J77" s="55"/>
       <c r="K77" s="98"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A78" s="71" t="s">
         <v>211</v>
       </c>
@@ -14180,7 +14230,7 @@
       </c>
       <c r="K78" s="97"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A79" s="71" t="s">
         <v>212</v>
       </c>
@@ -14207,7 +14257,7 @@
         <v>0.93680161201685286</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A80" s="71" t="s">
         <v>213</v>
       </c>
@@ -14234,7 +14284,7 @@
         <v>0.93292760238366934</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A81" s="71" t="s">
         <v>214</v>
       </c>
@@ -14261,7 +14311,7 @@
         <v>0.96554227633195577</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A82" s="71" t="s">
         <v>399</v>
       </c>
@@ -14288,7 +14338,7 @@
         <v>0.93359512366662756</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A83" s="99" t="s">
         <v>215</v>
       </c>
@@ -14311,7 +14361,7 @@
       </c>
       <c r="I83" s="102"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A84" s="103" t="s">
         <v>216</v>
       </c>
@@ -14334,7 +14384,7 @@
         <v>0.85292563033160751</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A85" s="103" t="s">
         <v>217</v>
       </c>
@@ -14357,7 +14407,7 @@
         <v>0.88047037071579148</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A86" s="103" t="s">
         <v>218</v>
       </c>
@@ -14384,7 +14434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A87" s="106" t="s">
         <v>219</v>
       </c>
@@ -14411,7 +14461,7 @@
         <v>0.90447216306662592</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A88" s="107" t="s">
         <v>220</v>
       </c>
@@ -14438,7 +14488,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:14" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A89" s="73" t="s">
         <v>221</v>
       </c>
@@ -14465,7 +14515,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A90" s="23" t="s">
         <v>222</v>
       </c>
@@ -14492,7 +14542,7 @@
         <v>0.8252427184466018</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A91" s="73" t="s">
         <v>223</v>
       </c>
@@ -14519,7 +14569,7 @@
         <v>0.87681159420289856</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A92" s="118" t="s">
         <v>400</v>
       </c>
@@ -14553,7 +14603,7 @@
       <c r="M92" s="121"/>
       <c r="N92" s="122"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A93" s="123" t="s">
         <v>401</v>
       </c>
@@ -14579,12 +14629,12 @@
       <c r="M93" s="125"/>
       <c r="N93" s="126"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A94" s="127"/>
       <c r="B94" s="128"/>
       <c r="N94" s="129"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A95" s="127" t="s">
         <v>224</v>
       </c>
@@ -14599,7 +14649,7 @@
       <c r="M95" s="73"/>
       <c r="N95" s="129"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A96" s="130" t="s">
         <v>225</v>
       </c>
@@ -14617,7 +14667,7 @@
       <c r="M96" s="133"/>
       <c r="N96" s="134"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A97" s="135" t="s">
         <v>226</v>
       </c>
@@ -14661,7 +14711,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A98" s="136" t="s">
         <v>233</v>
       </c>
@@ -14705,7 +14755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A99" s="137" t="s">
         <v>234</v>
       </c>
@@ -14749,7 +14799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A100" s="123" t="s">
         <v>235</v>
       </c>
@@ -14793,7 +14843,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A101" s="127" t="s">
         <v>236</v>
       </c>
@@ -14837,13 +14887,13 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A102" s="127"/>
       <c r="B102" s="128"/>
       <c r="F102" s="73"/>
       <c r="G102" s="129"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A103" s="127" t="s">
         <v>237</v>
       </c>
@@ -14852,7 +14902,7 @@
       <c r="F103" s="73"/>
       <c r="G103" s="129"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A104" s="127" t="s">
         <v>238</v>
       </c>
@@ -14875,7 +14925,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A105" s="130" t="s">
         <v>233</v>
       </c>
@@ -14896,7 +14946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A106" s="22" t="s">
         <v>242</v>
       </c>
@@ -14919,7 +14969,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A107" s="23" t="s">
         <v>243</v>
       </c>
@@ -14942,7 +14992,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A108" s="118" t="s">
         <v>244</v>
       </c>
@@ -14965,7 +15015,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A109" s="127" t="s">
         <v>245</v>
       </c>
@@ -14988,7 +15038,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A110" s="127" t="s">
         <v>246</v>
       </c>
@@ -15011,17 +15061,17 @@
         <v>-71</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A111" s="127"/>
       <c r="B111" s="146"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A112" s="130" t="s">
         <v>247</v>
       </c>
       <c r="B112" s="147"/>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A113" s="22" t="s">
         <v>248</v>
       </c>
@@ -15029,7 +15079,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A114" s="148" t="s">
         <v>249</v>
       </c>
@@ -15039,7 +15089,7 @@
       <c r="C114" s="73"/>
       <c r="D114" s="73"/>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A115" s="73" t="s">
         <v>250</v>
       </c>
@@ -15047,7 +15097,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A116" s="22" t="s">
         <v>251</v>
       </c>
@@ -15060,7 +15110,7 @@
       <c r="R116" s="151"/>
       <c r="V116" s="151"/>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A117" s="22" t="s">
         <v>252</v>
       </c>
@@ -15073,7 +15123,7 @@
       <c r="R117" s="154"/>
       <c r="V117" s="154"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B118" s="155"/>
       <c r="C118" s="156"/>
       <c r="D118" s="157"/>
@@ -15093,7 +15143,7 @@
       <c r="W118" s="158"/>
       <c r="X118" s="157"/>
     </row>
-    <row r="119" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A119" s="73" t="s">
         <v>253</v>
       </c>
@@ -15116,7 +15166,7 @@
       <c r="W119" s="160"/>
       <c r="X119" s="161"/>
     </row>
-    <row r="120" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B120" s="162"/>
       <c r="C120" s="163"/>
       <c r="D120" s="164"/>
@@ -15136,7 +15186,7 @@
       <c r="W120" s="163"/>
       <c r="X120" s="164"/>
     </row>
-    <row r="121" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B121" s="162">
         <v>10</v>
       </c>
@@ -15168,7 +15218,7 @@
       <c r="W121" s="163"/>
       <c r="X121" s="164"/>
     </row>
-    <row r="122" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B122" s="162">
         <v>10</v>
       </c>
@@ -15200,7 +15250,7 @@
       <c r="W122" s="163"/>
       <c r="X122" s="164"/>
     </row>
-    <row r="123" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B123" s="162" t="s">
         <v>254</v>
       </c>
@@ -15256,7 +15306,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B124" s="162">
         <v>1990</v>
       </c>
@@ -15312,7 +15362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B125" s="162">
         <v>1995</v>
       </c>
@@ -15368,7 +15418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B126" s="168">
         <v>2000</v>
       </c>
@@ -15424,7 +15474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B127" s="22">
         <v>2005</v>
       </c>
@@ -15480,7 +15530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A128" s="148"/>
       <c r="B128" s="22">
         <v>2010</v>
@@ -15537,7 +15587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A129" s="171"/>
       <c r="B129" s="172">
         <v>2015</v>
@@ -15595,7 +15645,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A130" s="175"/>
       <c r="B130" s="176">
         <v>2017</v>
@@ -15653,7 +15703,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A131" s="175"/>
       <c r="B131" s="179">
         <v>2020</v>
@@ -15669,7 +15719,7 @@
       <c r="G131" s="174"/>
       <c r="H131" s="174"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A132" s="175"/>
       <c r="B132" s="179"/>
       <c r="C132" s="179"/>
@@ -15679,7 +15729,7 @@
       <c r="G132" s="174"/>
       <c r="H132" s="174"/>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A133" s="175" t="s">
         <v>262</v>
       </c>
@@ -15691,7 +15741,7 @@
       <c r="G133" s="174"/>
       <c r="H133" s="174"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A134" s="181" t="s">
         <v>263</v>
       </c>
@@ -15713,7 +15763,7 @@
       <c r="G134" s="174"/>
       <c r="H134" s="174"/>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A135" s="174" t="s">
         <v>269</v>
       </c>
@@ -15735,7 +15785,7 @@
       <c r="G135" s="174"/>
       <c r="H135" s="174"/>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A136" s="171" t="s">
         <v>270</v>
       </c>
@@ -15757,7 +15807,7 @@
       <c r="G136" s="174"/>
       <c r="H136" s="174"/>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A137" s="175" t="s">
         <v>271</v>
       </c>
@@ -15779,7 +15829,7 @@
       <c r="G137" s="174"/>
       <c r="H137" s="174"/>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A138" s="175" t="s">
         <v>272</v>
       </c>
@@ -15801,7 +15851,7 @@
       <c r="G138" s="174"/>
       <c r="H138" s="174"/>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A139" s="175" t="s">
         <v>273</v>
       </c>
@@ -15823,7 +15873,7 @@
       <c r="G139" s="174"/>
       <c r="H139" s="174"/>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A140" s="175"/>
       <c r="B140" s="163"/>
       <c r="C140" s="179"/>
@@ -15833,7 +15883,7 @@
       <c r="G140" s="174"/>
       <c r="H140" s="174"/>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A141" s="181" t="s">
         <v>274</v>
       </c>
@@ -15855,7 +15905,7 @@
       <c r="G141" s="174"/>
       <c r="H141" s="174"/>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A142" s="174" t="s">
         <v>280</v>
       </c>
@@ -15877,7 +15927,7 @@
       <c r="G142" s="174"/>
       <c r="H142" s="174"/>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A143" s="171" t="s">
         <v>281</v>
       </c>
@@ -15900,7 +15950,7 @@
       <c r="H143" s="172"/>
       <c r="I143" s="190"/>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A144" s="175" t="s">
         <v>282</v>
       </c>
@@ -15923,7 +15973,7 @@
       <c r="H144" s="176"/>
       <c r="I144" s="129"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A145" s="175" t="s">
         <v>283</v>
       </c>
@@ -15946,7 +15996,7 @@
       <c r="H145" s="176"/>
       <c r="I145" s="129"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A146" s="175" t="s">
         <v>284</v>
       </c>
@@ -15969,7 +16019,7 @@
       <c r="H146" s="176"/>
       <c r="I146" s="129"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A147" s="175"/>
       <c r="B147" s="179"/>
       <c r="C147" s="177"/>
@@ -15980,7 +16030,7 @@
       <c r="H147" s="176"/>
       <c r="I147" s="129"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A148" s="175" t="s">
         <v>285</v>
       </c>
@@ -16009,7 +16059,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A149" s="175" t="s">
         <v>294</v>
       </c>
@@ -16038,7 +16088,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A150" s="175" t="s">
         <v>295</v>
       </c>
@@ -16067,7 +16117,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A151" s="195" t="s">
         <v>296</v>
       </c>
@@ -16096,7 +16146,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A152" s="22" t="s">
         <v>297</v>
       </c>
@@ -16125,7 +16175,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A153" s="22" t="s">
         <v>298</v>
       </c>
@@ -16154,7 +16204,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A154" s="22" t="s">
         <v>299</v>
       </c>
@@ -16183,7 +16233,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A155" s="22" t="s">
         <v>300</v>
       </c>
@@ -16212,7 +16262,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A156" s="22" t="s">
         <v>301</v>
       </c>
@@ -16241,7 +16291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A158" s="22" t="s">
         <v>402</v>
       </c>
@@ -16261,7 +16311,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A159" s="22" t="s">
         <v>403</v>
       </c>
@@ -16281,7 +16331,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A160" s="22" t="s">
         <v>404</v>
       </c>
@@ -16301,7 +16351,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A161" s="22" t="s">
         <v>405</v>
       </c>
@@ -16321,7 +16371,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A162" s="22" t="s">
         <v>406</v>
       </c>
@@ -16341,7 +16391,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A163" s="22" t="s">
         <v>407</v>
       </c>
@@ -16363,19 +16413,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$D$100:$E$100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"None, GWP, GTP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>$C$93:$D$93</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"AR5/GWP,AR5/GTP,AR4/GWP,AR3/GWP,AR2/GWP,AR1/GWP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>"1,2"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16385,17 +16435,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="U7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:AI22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="30.86328125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -16404,7 +16454,7 @@
     <col min="31" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>393</v>
       </c>
@@ -16511,7 +16561,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>340</v>
       </c>
@@ -16652,7 +16702,7 @@
         <v>3412141479896.8999</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -16793,7 +16843,7 @@
         <v>25306715975902.305</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -16934,7 +16984,7 @@
         <v>36953476200000</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A5" s="200" t="s">
         <v>335</v>
       </c>
@@ -17075,7 +17125,7 @@
         <v>39652608749183</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>336</v>
       </c>
@@ -17182,7 +17232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>337</v>
       </c>
@@ -17289,7 +17339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>338</v>
       </c>
@@ -17396,7 +17446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A9" s="200" t="s">
         <v>324</v>
       </c>
@@ -17537,7 +17587,7 @@
         <v>16244049954440</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>325</v>
       </c>
@@ -17678,7 +17728,7 @@
         <v>5023036000000</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A11" s="2" t="s">
         <v>326</v>
       </c>
@@ -17819,7 +17869,7 @@
         <v>5825000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A12" s="2" t="s">
         <v>327</v>
       </c>
@@ -17960,7 +18010,7 @@
         <v>3989233000000</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A13" s="2" t="s">
         <v>328</v>
       </c>
@@ -18101,7 +18151,7 @@
         <v>5359000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A14" s="2" t="s">
         <v>362</v>
       </c>
@@ -18242,7 +18292,7 @@
         <v>5670000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A15" s="2" t="s">
         <v>341</v>
       </c>
@@ -18383,7 +18433,7 @@
         <v>3412141479896.8999</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A16" s="2" t="s">
         <v>339</v>
       </c>
@@ -18490,7 +18540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>329</v>
       </c>
@@ -18631,7 +18681,7 @@
         <v>11279023225214.885</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>358</v>
       </c>
@@ -18772,7 +18822,7 @@
         <v>5676202000000</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>359</v>
       </c>
@@ -18913,7 +18963,7 @@
         <v>6287000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A20" s="200" t="s">
         <v>360</v>
       </c>
@@ -19054,7 +19104,7 @@
         <v>346024492638</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A21" s="200" t="s">
         <v>361</v>
       </c>
@@ -19195,7 +19245,7 @@
         <v>12322693643480.453</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>357</v>
       </c>
@@ -19342,24 +19392,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="U7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:AI22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="30.86328125" style="2" customWidth="1"/>
     <col min="2" max="35" width="10" style="2" customWidth="1"/>
     <col min="36" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>394</v>
       </c>
@@ -19466,7 +19516,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" s="200" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="200" t="s">
         <v>345</v>
       </c>
@@ -19607,7 +19657,7 @@
         <v>3412141.4798968998</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>322</v>
       </c>
@@ -19748,148 +19798,148 @@
         <v>25306715.975902304</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>323</v>
       </c>
       <c r="B4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="C4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="D4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="E4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="F4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="G4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="H4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="I4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="J4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="K4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="L4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="M4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="N4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="O4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="P4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="Q4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="R4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="S4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="T4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="U4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="V4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="W4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="X4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="Y4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="Z4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AA4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AB4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AC4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AD4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AE4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AF4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AG4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AH4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
       </c>
       <c r="AI4" s="5">
-        <f>'EU Calorific Values Natural Gas'!$C$11</f>
-        <v>3412141.4798968998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+        <f>'EU Calorific Values Natural Gas'!$C$10*'EU Calorific Values Natural Gas'!$D$13</f>
+        <v>3.6953476199999996E+19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A5" s="200" t="s">
         <v>349</v>
       </c>
@@ -20030,7 +20080,7 @@
         <v>39652608749.182999</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>336</v>
       </c>
@@ -20137,7 +20187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>337</v>
       </c>
@@ -20244,7 +20294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>338</v>
       </c>
@@ -20351,7 +20401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A9" s="200" t="s">
         <v>324</v>
       </c>
@@ -20492,7 +20542,7 @@
         <v>16244049.954440001</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A10" s="200" t="s">
         <v>325</v>
       </c>
@@ -20633,7 +20683,7 @@
         <v>31593.945799528399</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A11" s="200" t="s">
         <v>326</v>
       </c>
@@ -20774,7 +20824,7 @@
         <v>36638.147582906618</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A12" s="200" t="s">
         <v>327</v>
       </c>
@@ -20915,7 +20965,7 @@
         <v>25091.520583107522</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A13" s="200" t="s">
         <v>328</v>
       </c>
@@ -21056,7 +21106,7 @@
         <v>33707.095776274087</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A14" s="200" t="s">
         <v>362</v>
       </c>
@@ -21197,7 +21247,7 @@
         <v>35663.226917610395</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A15" s="2" t="s">
         <v>346</v>
       </c>
@@ -21338,7 +21388,7 @@
         <v>3412141.4798968998</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A16" s="2" t="s">
         <v>339</v>
       </c>
@@ -21445,7 +21495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A17" s="2" t="s">
         <v>329</v>
       </c>
@@ -21586,7 +21636,7 @@
         <v>11279023.225214886</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A18" s="2" t="s">
         <v>358</v>
       </c>
@@ -21727,7 +21777,7 @@
         <v>5676202</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A19" s="2" t="s">
         <v>359</v>
       </c>
@@ -21868,7 +21918,7 @@
         <v>6287000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A20" s="200" t="s">
         <v>360</v>
       </c>
@@ -22009,7 +22059,7 @@
         <v>24147.967203990858</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A21" s="200" t="s">
         <v>361</v>
       </c>
@@ -22150,7 +22200,7 @@
         <v>12322693.643480454</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A22" s="2" t="s">
         <v>357</v>
       </c>
@@ -22297,23 +22347,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="38.265625" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
     <col min="2" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>392</v>
       </c>
@@ -22420,7 +22470,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>310</v>
       </c>
@@ -22527,7 +22577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>311</v>
       </c>
@@ -22634,7 +22684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -22775,7 +22825,7 @@
         <v>1.9667413265602716E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -22916,7 +22966,7 @@
         <v>1.695967808755365E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -23023,7 +23073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>313</v>
       </c>
@@ -23130,7 +23180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>319</v>
       </c>
@@ -23271,7 +23321,7 @@
         <v>1.7423302444444446E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>391</v>
       </c>
@@ -23378,7 +23428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>360</v>
       </c>
@@ -23485,7 +23535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>357</v>
       </c>
@@ -23592,7 +23642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
       <c r="C15" s="6"/>
     </row>
   </sheetData>
@@ -23601,7 +23651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -23611,14 +23661,14 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>455</v>
       </c>

</xml_diff>

<commit_message>
Correct missing hydrogen conversion data
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26D93D-863D-41A0-A528-CA04EC9C5A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FEC962-1F1E-4854-B74F-884173F60F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3873,10 +3873,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="55">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4311,41 +4311,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4354,147 +4354,147 @@
       </c>
       <c r="C6" s="177"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="173" t="s">
         <v>395</v>
       </c>
       <c r="C13" s="177"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="174" t="s">
         <v>330</v>
       </c>
       <c r="B40" s="175"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>344</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="176" t="s">
         <v>386</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>323</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="176" t="s">
         <v>382</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="176" t="s">
         <v>384</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="176" t="s">
         <v>351</v>
       </c>
@@ -4556,16 +4556,16 @@
         <v>355</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="176"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="174" t="s">
         <v>333</v>
       </c>
       <c r="B49" s="175"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>344</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="176" t="s">
         <v>386</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>323</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>361</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="176" t="s">
         <v>385</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="176" t="s">
         <v>383</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="176" t="s">
         <v>349</v>
       </c>
@@ -4621,33 +4621,33 @@
         <v>350</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="174" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="174" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="173" t="s">
         <v>316</v>
       </c>
       <c r="B65" s="177"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>42</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3412000</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0.90718500000000002</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3.7854100000000002</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>235.215</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>159</v>
       </c>
@@ -4713,14 +4713,14 @@
       <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="20.88671875" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="16" t="s">
         <v>381</v>
       </c>
@@ -4827,8 +4827,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="18" t="s">
         <v>121</v>
       </c>
@@ -4839,7 +4839,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="18" t="s">
         <v>120</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="18" t="s">
         <v>118</v>
       </c>
@@ -4863,7 +4863,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="18" t="s">
         <v>117</v>
       </c>
@@ -4874,7 +4874,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>116</v>
       </c>
@@ -4882,12 +4882,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>2</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>2</v>
       </c>
@@ -5107,17 +5107,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>114</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>113</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>112</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>111</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>110</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>109</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>108</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>107</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>106</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>105</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>103</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>102</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>99</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>98</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>97</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>96</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>95</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>-2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>374</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>372</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>94</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>93</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>92</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>91</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>90</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>89</v>
       </c>
@@ -8168,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>88</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>87</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>-4.8299999999999998E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>86</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>-3.1150000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
@@ -8620,12 +8620,12 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>84</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>-2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>83</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>-3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>81</v>
       </c>
@@ -9077,12 +9077,12 @@
         <v>-2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>80</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>79</v>
       </c>
@@ -9308,7 +9308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>78</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>77</v>
       </c>
@@ -9534,7 +9534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>76</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>75</v>
       </c>
@@ -9760,7 +9760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>74</v>
       </c>
@@ -9873,12 +9873,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>73</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>-1.4100000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>72</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>-1.0139999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>71</v>
       </c>
@@ -10217,7 +10217,7 @@
         <v>-2.1699999999999999E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>70</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>2.8499999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>69</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>68</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>-5.5000000000000002E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>67</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>-9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>66</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>65</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>5.7700000000000004E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>64</v>
       </c>
@@ -11008,7 +11008,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>63</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>62</v>
       </c>
@@ -11234,7 +11234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>61</v>
       </c>
@@ -11347,78 +11347,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="182" t="s">
+    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="182"/>
-      <c r="D78" s="182"/>
-      <c r="E78" s="182"/>
-      <c r="F78" s="182"/>
-      <c r="G78" s="182"/>
-      <c r="H78" s="182"/>
-      <c r="I78" s="182"/>
-      <c r="J78" s="182"/>
-      <c r="K78" s="182"/>
-      <c r="L78" s="182"/>
-      <c r="M78" s="182"/>
-      <c r="N78" s="182"/>
-      <c r="O78" s="182"/>
-      <c r="P78" s="182"/>
-      <c r="Q78" s="182"/>
-      <c r="R78" s="182"/>
-      <c r="S78" s="182"/>
-      <c r="T78" s="182"/>
-      <c r="U78" s="182"/>
-      <c r="V78" s="182"/>
-      <c r="W78" s="182"/>
-      <c r="X78" s="182"/>
-      <c r="Y78" s="182"/>
-      <c r="Z78" s="182"/>
-      <c r="AA78" s="182"/>
-      <c r="AB78" s="182"/>
-      <c r="AC78" s="182"/>
-      <c r="AD78" s="182"/>
-      <c r="AE78" s="182"/>
-      <c r="AF78" s="182"/>
-      <c r="AG78" s="182"/>
-      <c r="AH78" s="182"/>
-      <c r="AI78" s="182"/>
-      <c r="AJ78" s="182"/>
-      <c r="AK78" s="182"/>
-    </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="183"/>
+      <c r="D78" s="183"/>
+      <c r="E78" s="183"/>
+      <c r="F78" s="183"/>
+      <c r="G78" s="183"/>
+      <c r="H78" s="183"/>
+      <c r="I78" s="183"/>
+      <c r="J78" s="183"/>
+      <c r="K78" s="183"/>
+      <c r="L78" s="183"/>
+      <c r="M78" s="183"/>
+      <c r="N78" s="183"/>
+      <c r="O78" s="183"/>
+      <c r="P78" s="183"/>
+      <c r="Q78" s="183"/>
+      <c r="R78" s="183"/>
+      <c r="S78" s="183"/>
+      <c r="T78" s="183"/>
+      <c r="U78" s="183"/>
+      <c r="V78" s="183"/>
+      <c r="W78" s="183"/>
+      <c r="X78" s="183"/>
+      <c r="Y78" s="183"/>
+      <c r="Z78" s="183"/>
+      <c r="AA78" s="183"/>
+      <c r="AB78" s="183"/>
+      <c r="AC78" s="183"/>
+      <c r="AD78" s="183"/>
+      <c r="AE78" s="183"/>
+      <c r="AF78" s="183"/>
+      <c r="AG78" s="183"/>
+      <c r="AH78" s="183"/>
+      <c r="AI78" s="183"/>
+      <c r="AJ78" s="183"/>
+      <c r="AK78" s="183"/>
+    </row>
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="s">
         <v>367</v>
       </c>
@@ -11436,39 +11436,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X163"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>126</v>
       </c>
@@ -11491,7 +11491,7 @@
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
         <v>302</v>
@@ -11516,7 +11516,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>137</v>
       </c>
@@ -11533,7 +11533,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>139</v>
       </c>
@@ -11554,7 +11554,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="40"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
         <v>142</v>
       </c>
@@ -11583,7 +11583,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
         <v>143</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
         <v>144</v>
       </c>
@@ -11641,7 +11641,7 @@
         <v>0.93500000000000016</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
         <v>145</v>
       </c>
@@ -11670,7 +11670,7 @@
         <v>0.93500000000000016</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
         <v>146</v>
       </c>
@@ -11707,7 +11707,7 @@
       <c r="R11" s="46"/>
       <c r="S11" s="52"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>147</v>
       </c>
@@ -11736,7 +11736,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -11765,7 +11765,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -11794,7 +11794,7 @@
         <v>0.93726057101554017</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
         <v>150</v>
       </c>
@@ -11831,7 +11831,7 @@
       <c r="V15" s="57"/>
       <c r="W15" s="53"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="41" t="s">
         <v>151</v>
       </c>
@@ -11865,7 +11865,7 @@
       <c r="V16" s="57"/>
       <c r="W16" s="53"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
         <v>152</v>
       </c>
@@ -11902,7 +11902,7 @@
       <c r="V17" s="57"/>
       <c r="W17" s="53"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="41" t="s">
         <v>153</v>
       </c>
@@ -11936,7 +11936,7 @@
       <c r="V18" s="57"/>
       <c r="W18" s="53"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="41" t="s">
         <v>154</v>
       </c>
@@ -11970,7 +11970,7 @@
       <c r="M19" s="57"/>
       <c r="N19" s="53"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="41" t="s">
         <v>303</v>
       </c>
@@ -12000,7 +12000,7 @@
       </c>
       <c r="W20" s="53"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="59" t="s">
         <v>400</v>
       </c>
@@ -12027,7 +12027,7 @@
       </c>
       <c r="I21" s="47"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
         <v>155</v>
       </c>
@@ -12056,7 +12056,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="41" t="s">
         <v>156</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="41" t="s">
         <v>157</v>
       </c>
@@ -12114,7 +12114,7 @@
         <v>0.93476175247841387</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
         <v>401</v>
       </c>
@@ -12143,7 +12143,7 @@
         <v>0.93404711473172097</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="41" t="s">
         <v>158</v>
       </c>
@@ -12172,7 +12172,7 @@
         <v>0.93500003751584637</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>159</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>160</v>
       </c>
@@ -12230,7 +12230,7 @@
         <v>0.93135126106564226</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>161</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
         <v>162</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
         <v>163</v>
       </c>
@@ -12317,7 +12317,7 @@
         <v>0.87806748466257667</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
         <v>164</v>
       </c>
@@ -12346,7 +12346,7 @@
         <v>0.90299302022950434</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>165</v>
       </c>
@@ -12375,7 +12375,7 @@
         <v>0.92051300964428628</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="41" t="s">
         <v>166</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>0.92867915675168411</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="41" t="s">
         <v>167</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>0.93364967025896739</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="41" t="s">
         <v>168</v>
       </c>
@@ -12462,7 +12462,7 @@
         <v>0.9293293950333662</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
         <v>169</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>0.88092431030417351</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
         <v>170</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>0.91165189789710355</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>171</v>
       </c>
@@ -12549,7 +12549,7 @@
         <v>0.91165189789710355</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
         <v>172</v>
       </c>
@@ -12578,7 +12578,7 @@
         <v>0.93427633635511098</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
         <v>173</v>
       </c>
@@ -12607,7 +12607,7 @@
         <v>0.95108821041298164</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>174</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>0.93427633635511098</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>175</v>
       </c>
@@ -12665,7 +12665,7 @@
         <v>0.93938096730547249</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="41" t="s">
         <v>176</v>
       </c>
@@ -12694,7 +12694,7 @@
         <v>0.92840083590406852</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -12723,7 +12723,7 @@
         <v>0.93361506882395562</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="41" t="s">
         <v>178</v>
       </c>
@@ -12752,7 +12752,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="41" t="s">
         <v>402</v>
       </c>
@@ -12781,7 +12781,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="41" t="s">
         <v>179</v>
       </c>
@@ -12810,7 +12810,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="41" t="s">
         <v>180</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>0.84675180455302612</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="41" t="s">
         <v>181</v>
       </c>
@@ -12868,7 +12868,7 @@
         <v>0.92494808662118067</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="41" t="s">
         <v>182</v>
       </c>
@@ -12897,7 +12897,7 @@
         <v>0.92528460728977324</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="41" t="s">
         <v>183</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>0.92548586165607438</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="41" t="s">
         <v>184</v>
       </c>
@@ -12955,7 +12955,7 @@
         <v>0.92007362914163926</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="41" t="s">
         <v>185</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>0.91375811688311692</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="41" t="s">
         <v>186</v>
       </c>
@@ -13013,7 +13013,7 @@
         <v>0.92923017182797785</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="41" t="s">
         <v>187</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>0.92157077225989936</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="41" t="s">
         <v>188</v>
       </c>
@@ -13069,7 +13069,7 @@
         <v>0.92932939503336609</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="36" t="s">
         <v>189</v>
       </c>
@@ -13098,7 +13098,7 @@
         <v>0.93722267739953979</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="41" t="s">
         <v>191</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="41" t="s">
         <v>194</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>0.90266299357208446</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="41" t="s">
         <v>195</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>0.9009009009009008</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="41" t="s">
         <v>196</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>0.84548104956268222</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="41" t="s">
         <v>197</v>
       </c>
@@ -13229,7 +13229,7 @@
       </c>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="36" t="s">
         <v>190</v>
       </c>
@@ -13258,7 +13258,7 @@
         <v>0.90586790472651468</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="41" t="s">
         <v>198</v>
       </c>
@@ -13279,7 +13279,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="59" t="s">
         <v>200</v>
       </c>
@@ -13305,7 +13305,7 @@
       <c r="I66" s="81"/>
       <c r="K66" s="82"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="59" t="s">
         <v>201</v>
       </c>
@@ -13333,7 +13333,7 @@
       </c>
       <c r="K67" s="82"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="59" t="s">
         <v>202</v>
       </c>
@@ -13361,7 +13361,7 @@
       </c>
       <c r="K68" s="82"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="59" t="s">
         <v>203</v>
       </c>
@@ -13389,7 +13389,7 @@
       </c>
       <c r="K69" s="82"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="59" t="s">
         <v>204</v>
       </c>
@@ -13417,7 +13417,7 @@
       </c>
       <c r="K70" s="82"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="41" t="s">
         <v>205</v>
       </c>
@@ -13446,7 +13446,7 @@
       <c r="K71" s="82"/>
       <c r="L71" s="82"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="41" t="s">
         <v>206</v>
       </c>
@@ -13474,7 +13474,7 @@
       </c>
       <c r="K72" s="82"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="41" t="s">
         <v>207</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>0.94242199100000001</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="41" t="s">
         <v>208</v>
       </c>
@@ -13529,7 +13529,7 @@
       </c>
       <c r="K74" s="84"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="41" t="s">
         <v>403</v>
       </c>
@@ -13557,7 +13557,7 @@
       </c>
       <c r="K75" s="84"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="41" t="s">
         <v>209</v>
       </c>
@@ -13584,7 +13584,7 @@
         <v>0.93173565722585328</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="41" t="s">
         <v>210</v>
       </c>
@@ -13612,7 +13612,7 @@
       </c>
       <c r="K77" s="85"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="41" t="s">
         <v>211</v>
       </c>
@@ -13640,7 +13640,7 @@
       </c>
       <c r="K78" s="84"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="41" t="s">
         <v>212</v>
       </c>
@@ -13667,7 +13667,7 @@
         <v>0.93680161201685286</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="41" t="s">
         <v>213</v>
       </c>
@@ -13694,7 +13694,7 @@
         <v>0.93292760238366934</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="41" t="s">
         <v>214</v>
       </c>
@@ -13721,7 +13721,7 @@
         <v>0.96554227633195577</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="41" t="s">
         <v>404</v>
       </c>
@@ -13748,7 +13748,7 @@
         <v>0.93359512366662756</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="59" t="s">
         <v>215</v>
       </c>
@@ -13771,7 +13771,7 @@
       </c>
       <c r="I83" s="88"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="89" t="s">
         <v>216</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>0.85292563033160751</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="89" t="s">
         <v>217</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>0.88047037071579148</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="89" t="s">
         <v>218</v>
       </c>
@@ -13844,7 +13844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="92" t="s">
         <v>219</v>
       </c>
@@ -13871,7 +13871,7 @@
         <v>0.90447216306662592</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="93" t="s">
         <v>220</v>
       </c>
@@ -13898,7 +13898,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>221</v>
       </c>
@@ -13925,7 +13925,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="20" t="s">
         <v>222</v>
       </c>
@@ -13952,7 +13952,7 @@
         <v>0.8252427184466018</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -13979,7 +13979,7 @@
         <v>0.87681159420289856</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="104" t="s">
         <v>405</v>
       </c>
@@ -14013,7 +14013,7 @@
       <c r="M92" s="107"/>
       <c r="N92" s="108"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="109" t="s">
         <v>406</v>
       </c>
@@ -14039,19 +14039,19 @@
       <c r="M93" s="111"/>
       <c r="N93" s="112"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="113"/>
       <c r="B94" s="114"/>
       <c r="N94" s="115"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="113" t="s">
         <v>224</v>
       </c>
       <c r="B95" s="114"/>
       <c r="N95" s="115"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="109" t="s">
         <v>225</v>
       </c>
@@ -14069,7 +14069,7 @@
       <c r="M96" s="117"/>
       <c r="N96" s="118"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="119" t="s">
         <v>226</v>
       </c>
@@ -14113,7 +14113,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>233</v>
       </c>
@@ -14157,7 +14157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="120" t="s">
         <v>234</v>
       </c>
@@ -14201,7 +14201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="109" t="s">
         <v>235</v>
       </c>
@@ -14245,7 +14245,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="113" t="s">
         <v>236</v>
       </c>
@@ -14289,19 +14289,19 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="113"/>
       <c r="B102" s="114"/>
       <c r="G102" s="115"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="113" t="s">
         <v>237</v>
       </c>
       <c r="B103" s="114"/>
       <c r="G103" s="115"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="113" t="s">
         <v>238</v>
       </c>
@@ -14324,7 +14324,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="109" t="s">
         <v>233</v>
       </c>
@@ -14345,7 +14345,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>242</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="20" t="s">
         <v>243</v>
       </c>
@@ -14391,7 +14391,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="104" t="s">
         <v>244</v>
       </c>
@@ -14414,7 +14414,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="113" t="s">
         <v>245</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="113" t="s">
         <v>246</v>
       </c>
@@ -14460,17 +14460,17 @@
         <v>-71</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="113"/>
       <c r="B111" s="129"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="109" t="s">
         <v>247</v>
       </c>
       <c r="B112" s="130"/>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>248</v>
       </c>
@@ -14478,7 +14478,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
         <v>249</v>
       </c>
@@ -14486,7 +14486,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>250</v>
       </c>
@@ -14494,7 +14494,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>251</v>
       </c>
@@ -14507,7 +14507,7 @@
       <c r="R116" s="133"/>
       <c r="V116" s="133"/>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>252</v>
       </c>
@@ -14520,7 +14520,7 @@
       <c r="R117" s="136"/>
       <c r="V117" s="136"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B118" s="137"/>
       <c r="C118" s="138"/>
       <c r="D118" s="139"/>
@@ -14540,7 +14540,7 @@
       <c r="W118" s="140"/>
       <c r="X118" s="139"/>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>253</v>
       </c>
@@ -14563,7 +14563,7 @@
       <c r="W119" s="142"/>
       <c r="X119" s="143"/>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B120" s="144"/>
       <c r="C120" s="136"/>
       <c r="D120" s="145"/>
@@ -14583,7 +14583,7 @@
       <c r="W120" s="136"/>
       <c r="X120" s="145"/>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B121" s="144">
         <v>10</v>
       </c>
@@ -14615,7 +14615,7 @@
       <c r="W121" s="136"/>
       <c r="X121" s="145"/>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B122" s="144">
         <v>10</v>
       </c>
@@ -14647,7 +14647,7 @@
       <c r="W122" s="136"/>
       <c r="X122" s="145"/>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B123" s="144" t="s">
         <v>254</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B124" s="144">
         <v>1990</v>
       </c>
@@ -14759,7 +14759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B125" s="144">
         <v>1995</v>
       </c>
@@ -14815,7 +14815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B126" s="149">
         <v>2000</v>
       </c>
@@ -14871,7 +14871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>2005</v>
       </c>
@@ -14927,7 +14927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A128" s="20"/>
       <c r="B128">
         <v>2010</v>
@@ -14984,7 +14984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129" s="152"/>
       <c r="B129" s="153">
         <v>2015</v>
@@ -15042,7 +15042,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130" s="155"/>
       <c r="B130" s="156">
         <v>2017</v>
@@ -15100,7 +15100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131" s="155"/>
       <c r="B131" s="159">
         <v>2020</v>
@@ -15114,7 +15114,7 @@
       <c r="E131" s="157"/>
       <c r="F131" s="160"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A132" s="155"/>
       <c r="B132" s="159"/>
       <c r="C132" s="159"/>
@@ -15122,7 +15122,7 @@
       <c r="E132" s="159"/>
       <c r="F132" s="160"/>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A133" s="155" t="s">
         <v>262</v>
       </c>
@@ -15132,7 +15132,7 @@
       <c r="E133" s="156"/>
       <c r="F133" s="158"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A134" s="161" t="s">
         <v>263</v>
       </c>
@@ -15152,7 +15152,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>269</v>
       </c>
@@ -15172,7 +15172,7 @@
         <v>907184.74</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A136" s="152" t="s">
         <v>270</v>
       </c>
@@ -15192,7 +15192,7 @@
         <v>907.18474000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A137" s="155" t="s">
         <v>271</v>
       </c>
@@ -15212,7 +15212,7 @@
         <v>0.90718474000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A138" s="155" t="s">
         <v>272</v>
       </c>
@@ -15232,7 +15232,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A139" s="155" t="s">
         <v>273</v>
       </c>
@@ -15252,7 +15252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A140" s="155"/>
       <c r="B140" s="136"/>
       <c r="C140" s="159"/>
@@ -15260,7 +15260,7 @@
       <c r="E140" s="156"/>
       <c r="F140" s="160"/>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A141" s="161" t="s">
         <v>274</v>
       </c>
@@ -15280,7 +15280,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -15300,7 +15300,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A143" s="152" t="s">
         <v>281</v>
       </c>
@@ -15323,7 +15323,7 @@
       <c r="H143" s="153"/>
       <c r="I143" s="154"/>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A144" s="155" t="s">
         <v>282</v>
       </c>
@@ -15346,7 +15346,7 @@
       <c r="H144" s="156"/>
       <c r="I144" s="115"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="155" t="s">
         <v>283</v>
       </c>
@@ -15369,7 +15369,7 @@
       <c r="H145" s="156"/>
       <c r="I145" s="115"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="155" t="s">
         <v>284</v>
       </c>
@@ -15392,7 +15392,7 @@
       <c r="H146" s="156"/>
       <c r="I146" s="115"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="155"/>
       <c r="B147" s="159"/>
       <c r="C147" s="157"/>
@@ -15403,7 +15403,7 @@
       <c r="H147" s="156"/>
       <c r="I147" s="115"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="155" t="s">
         <v>285</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="155" t="s">
         <v>294</v>
       </c>
@@ -15461,7 +15461,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="155" t="s">
         <v>295</v>
       </c>
@@ -15490,7 +15490,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="161" t="s">
         <v>296</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>297</v>
       </c>
@@ -15548,7 +15548,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>298</v>
       </c>
@@ -15577,7 +15577,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>299</v>
       </c>
@@ -15606,7 +15606,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>300</v>
       </c>
@@ -15635,7 +15635,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>301</v>
       </c>
@@ -15664,7 +15664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>407</v>
       </c>
@@ -15684,7 +15684,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>408</v>
       </c>
@@ -15704,7 +15704,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>409</v>
       </c>
@@ -15724,7 +15724,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>410</v>
       </c>
@@ -15744,7 +15744,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>411</v>
       </c>
@@ -15764,7 +15764,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>412</v>
       </c>
@@ -15818,14 +15818,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>398</v>
       </c>
@@ -15932,7 +15932,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>342</v>
       </c>
@@ -16073,7 +16073,7 @@
         <v>3412000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -16214,7 +16214,7 @@
         <v>21922192276106.859</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -16355,7 +16355,7 @@
         <v>1036999999999999.9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>336</v>
       </c>
@@ -16496,7 +16496,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -16603,7 +16603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>338</v>
       </c>
@@ -16710,7 +16710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>339</v>
       </c>
@@ -16817,7 +16817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -16958,7 +16958,7 @@
         <v>19737980676488.258</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>325</v>
       </c>
@@ -17099,7 +17099,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>326</v>
       </c>
@@ -17240,7 +17240,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>327</v>
       </c>
@@ -17381,7 +17381,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>328</v>
       </c>
@@ -17522,7 +17522,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>366</v>
       </c>
@@ -17663,7 +17663,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>343</v>
       </c>
@@ -17804,7 +17804,7 @@
         <v>3412000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>340</v>
       </c>
@@ -17911,7 +17911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>329</v>
       </c>
@@ -18052,7 +18052,7 @@
         <v>14321557313799.941</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>362</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>363</v>
       </c>
@@ -18334,7 +18334,7 @@
         <v>5810700000000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>364</v>
       </c>
@@ -18475,7 +18475,7 @@
         <v>24147978686.588772</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>365</v>
       </c>
@@ -18616,7 +18616,7 @@
         <v>14973180315221.879</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>361</v>
       </c>
@@ -18773,13 +18773,13 @@
       <selection activeCell="AF31" sqref="AF31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
     <col min="2" max="35" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>399</v>
       </c>
@@ -18886,7 +18886,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>347</v>
       </c>
@@ -19027,7 +19027,7 @@
         <v>3412000</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -19168,7 +19168,7 @@
         <v>21922192.276106857</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -19309,7 +19309,7 @@
         <v>1036999.9999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>353</v>
       </c>
@@ -19450,7 +19450,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -19557,7 +19557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>338</v>
       </c>
@@ -19664,7 +19664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>339</v>
       </c>
@@ -19771,7 +19771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -19912,7 +19912,7 @@
         <v>19737980.676488258</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>325</v>
       </c>
@@ -20053,7 +20053,7 @@
         <v>31591.421383647797</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>326</v>
       </c>
@@ -20194,7 +20194,7 @@
         <v>36635.220125786167</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>327</v>
       </c>
@@ -20335,7 +20335,7 @@
         <v>25089.515723270441</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>328</v>
       </c>
@@ -20476,7 +20476,7 @@
         <v>33704.402515723268</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>366</v>
       </c>
@@ -20617,7 +20617,7 @@
         <v>35660.377358490565</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>348</v>
       </c>
@@ -20758,7 +20758,7 @@
         <v>3412000</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>340</v>
       </c>
@@ -20865,7 +20865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>329</v>
       </c>
@@ -21006,7 +21006,7 @@
         <v>14321557.313799942</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>362</v>
       </c>
@@ -21147,7 +21147,7 @@
         <v>5810700</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>363</v>
       </c>
@@ -21288,7 +21288,7 @@
         <v>5810700</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>364</v>
       </c>
@@ -21429,7 +21429,7 @@
         <v>24147.978686588769</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>365</v>
       </c>
@@ -21570,7 +21570,7 @@
         <v>14973180.315221878</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>361</v>
       </c>
@@ -21727,13 +21727,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" customWidth="1"/>
     <col min="2" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>397</v>
       </c>
@@ -21840,7 +21840,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>310</v>
       </c>
@@ -21947,7 +21947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>311</v>
       </c>
@@ -22054,7 +22054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -22195,7 +22195,7 @@
         <v>31591.421383647797</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -22336,7 +22336,7 @@
         <v>36635.220125786167</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -22443,7 +22443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>313</v>
       </c>
@@ -22550,7 +22550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>319</v>
       </c>
@@ -22691,7 +22691,7 @@
         <v>35660.377358490565</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>394</v>
       </c>
@@ -22798,7 +22798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -22905,7 +22905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>361</v>
       </c>
@@ -23028,17 +23028,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -23063,24 +23063,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>CONVERT(About!A77,"kg","lbm")*1000000000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="183"/>
+        <f>'GREET1 Fuel_Specs'!D62/'GREET1 Fuel_Specs'!E62/1000/1000/1000/1000000</f>
+        <v>1.3450980392156863E-13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="182"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
for testing run FF55 and add a 100% RPS
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464E32CF-936F-463D-B954-A6EAACD9BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2462C1-FC5B-4026-900B-E45BAB03C4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31650" yWindow="1305" windowWidth="23955" windowHeight="15120" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4299,7 +4299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -11437,8 +11437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X163"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:H62"/>
+    <sheetView topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23026,7 +23026,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23060,8 +23060,8 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23076,8 +23076,8 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f>'GREET1 Fuel_Specs'!D62/'GREET1 Fuel_Specs'!E62/1000/1000/1000/1000000</f>
-        <v>1.3450980392156863E-13</v>
+        <f>'GREET1 Fuel_Specs'!D62/'GREET1 Fuel_Specs'!E62*10^12</f>
+        <v>134509803921568.64</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adjusting BCF - BpEIEOU need to check that this is coming out right in webtool - a little confusing
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB78AF76-6E56-4BA5-A53B-00C63AD54C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E628F9F-D913-4241-8DCF-C95AF55F19F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30330" yWindow="1560" windowWidth="20460" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30330" yWindow="1560" windowWidth="20460" windowHeight="13740" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4299,7 +4299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -18771,7 +18771,7 @@
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23025,8 +23025,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23044,8 +23044,7 @@
         <v>299</v>
       </c>
       <c r="B2">
-        <f>About!A67*10^6</f>
-        <v>3412000000000</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
webapp and unit conversion updates
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8349521C-220D-4079-8EE9-7EEA4F982B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A7B0C-1DAF-41DC-82B5-E7890000B631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30330" yWindow="1560" windowWidth="20460" windowHeight="13740" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35415" yWindow="3420" windowWidth="23520" windowHeight="11295" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2469,7 +2469,7 @@
     <t>gallons to TWh</t>
   </si>
   <si>
-    <t>Energy Import Export Output Unit (TWh/energy output unit)</t>
+    <t>Energy Import Export Output Unit (BTU/energy output unit)</t>
   </si>
 </sst>
 </file>
@@ -4297,10 +4297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4629,13 +4629,13 @@
         <v>343</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="173" t="s">
         <v>316</v>
       </c>
       <c r="B65" s="177"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>42</v>
       </c>
@@ -4643,15 +4643,16 @@
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3412000</v>
       </c>
       <c r="B67" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E67" s="181"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.90718500000000002</v>
       </c>
@@ -4659,7 +4660,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3.7854100000000002</v>
       </c>
@@ -4667,7 +4668,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>235.215</v>
       </c>
@@ -4675,7 +4676,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>159</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.6994</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>423</v>
       </c>
@@ -23026,7 +23027,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23041,10 +23042,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>343</v>
+        <v>299</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <f>About!A67*10^6</f>
+        <v>3412000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing units for H2 consumption from thousand metric tons to million metric tons, per agora's request
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9662C5CF-B525-409B-930A-D0E390971B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7F23C0-B395-4E71-BBA6-91EAD5A5CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35415" yWindow="3420" windowWidth="23520" windowHeight="11295" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="1920" windowWidth="21660" windowHeight="14205" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2352,9 +2352,6 @@
     <t>hard coal, lignite, biomass, municipal solid waste</t>
   </si>
   <si>
-    <t>thousand metric tons</t>
-  </si>
-  <si>
     <t>The Fuel Economy Output Unit is used to help compare fuel economy of different technologies of the same vehicle</t>
   </si>
   <si>
@@ -2439,9 +2436,6 @@
     <t>Short ton to MT</t>
   </si>
   <si>
-    <t>millions of metric tons</t>
-  </si>
-  <si>
     <t>gallons to liters</t>
   </si>
   <si>
@@ -2470,6 +2464,12 @@
   </si>
   <si>
     <t>Energy Import Export Output Unit (BTU/energy output unit)</t>
+  </si>
+  <si>
+    <t>million metric tons</t>
+  </si>
+  <si>
+    <t>millions metric tons</t>
   </si>
 </sst>
 </file>
@@ -4299,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4369,7 +4369,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C13" s="177"/>
     </row>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4415,32 +4415,32 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -4460,17 +4460,17 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4498,7 +4498,7 @@
         <v>384</v>
       </c>
       <c r="B42" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4514,7 +4514,7 @@
         <v>359</v>
       </c>
       <c r="B44" t="s">
-        <v>385</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>384</v>
       </c>
       <c r="B51" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -4616,7 +4616,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>0.90718500000000002</v>
       </c>
       <c r="B68" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>3.7854100000000002</v>
       </c>
       <c r="B69" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>235.215</v>
       </c>
       <c r="B70" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4681,7 +4681,7 @@
         <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4689,12 +4689,12 @@
         <v>1.6994</v>
       </c>
       <c r="B72" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -12004,7 +12004,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B21" s="42">
         <v>129487.84757606639</v>
@@ -12118,7 +12118,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B25" s="42">
         <v>118237.434842673</v>
@@ -12756,7 +12756,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B47" s="42">
         <v>112060.7</v>
@@ -13533,7 +13533,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B75" s="42">
         <v>28385750.368920002</v>
@@ -13725,7 +13725,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B82" s="42">
         <v>15929000</v>
@@ -13983,7 +13983,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="104" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B92" s="105">
         <v>152370.90134048002</v>
@@ -14017,7 +14017,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="109" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B93" s="110">
         <v>144230</v>
@@ -15668,27 +15668,27 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>403</v>
+      </c>
+      <c r="B158" t="s">
         <v>404</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>405</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" t="s">
         <v>406</v>
       </c>
-      <c r="D158" t="s">
+      <c r="E158" t="s">
         <v>407</v>
       </c>
-      <c r="E158" t="s">
+      <c r="F158" t="s">
         <v>408</v>
-      </c>
-      <c r="F158" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -15708,7 +15708,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B160">
         <v>1E-3</v>
@@ -15728,7 +15728,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B161">
         <v>9.9999999999999995E-7</v>
@@ -15748,7 +15748,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B162">
         <v>3.2808398950131233E-3</v>
@@ -15768,7 +15768,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B163">
         <v>6.2137273664980671E-7</v>
@@ -15817,7 +15817,7 @@
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15829,7 +15829,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -18623,140 +18623,140 @@
         <v>359</v>
       </c>
       <c r="B22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="C22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="D22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="E22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="F22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="G22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="H22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="I22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="J22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="K22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="L22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="M22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="N22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="O22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="P22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="Q22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="R22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="S22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="T22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="U22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="V22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="W22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="X22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="Y22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="Z22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AA22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AB22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AC22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AD22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AE22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AF22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AG22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AH22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
       <c r="AI22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
+        <v>134509803.92156866</v>
       </c>
     </row>
   </sheetData>
@@ -18772,7 +18772,7 @@
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18783,7 +18783,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -21737,7 +21737,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -22695,7 +22695,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -23026,8 +23026,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23037,7 +23037,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -23061,7 +23061,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -23072,7 +23072,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
additional work to change H2 units in webapp
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7F23C0-B395-4E71-BBA6-91EAD5A5CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15429309-1BA4-4EA0-AEDE-CA900DDC3245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="1920" windowWidth="21660" windowHeight="14205" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21660" windowHeight="14205" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4300,7 +4300,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15816,8 +15816,8 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18623,140 +18623,140 @@
         <v>359</v>
       </c>
       <c r="B22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="C22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="D22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="E22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="F22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="G22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="H22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="I22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="J22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="K22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="L22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="M22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="N22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="O22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="P22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="Q22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="R22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="S22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="T22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="U22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="V22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="W22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="X22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="Y22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="Z22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AA22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AB22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AC22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AD22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AE22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AF22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AG22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AH22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
       <c r="AI22" s="181">
-        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)/1000</f>
-        <v>134509803.92156866</v>
+        <f>('GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9)*1000</f>
+        <v>134509803921568.66</v>
       </c>
     </row>
   </sheetData>
@@ -23061,7 +23061,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>